<commit_message>
added links to user and updated scraped sites
</commit_message>
<xml_diff>
--- a/app/PickleJar/AllTimePickle.xlsx
+++ b/app/PickleJar/AllTimePickle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -936,6 +936,389 @@
       </c>
       <c r="H16" t="inlineStr"/>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Kanzlerkandidatin der Grünen</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Baerbock will Kurzstreckenflüge abschaffen</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>BERLIN - Nach SPD-Kanzlerkandidat Olaf Scholz hat auch Grünen-Kandidatin Annalena Baerbock angekündigt, Flugreisen im Fall einer Regierungsübernahme unattraktiver machen zu wollen. Im Interview mit der "Bild am Sonntag" machte sie deutlich, dass sie perspektivisch für die Abschaffung von Kurzstreckenflügen ist.»</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>www.aero.de/news-39649/Baerbock-will-Kurzstreckenfluege-abschaffen.html</t>
+        </is>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Italien Fliegertouren 2021</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Wir möchten nach der coronabedingten Pause nun endlich wieder mit Euch zu unseren wunderschönen und außergewöhnlichen Fliegertouren nach Italien abheben.
+Wir freuen uns sehr auf Eure Teilnahme und gemeinsame Flüge nach Italien, sowie wunderschöne Aufenthalte an den Destinationen!</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://air-munich.de/</t>
+        </is>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AZF Sprechfunkzeugnis</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Am 06. und 07. März findet der nächste Kurs für das AZF Sprechfunkzeugnis statt. Für weitere Infos und Anmeldungen bitte eine Email an: office@air-munich.de</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://air-munich.de/</t>
+        </is>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Breezer B400-6</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Unser Breezer B400-6 wurde im Breezer Werk in Bredstedt (Schleswig-Holstein) auf 600kg MTOM aufgerüstet, sowie mit einer elektrischen Trimmung ausgestattet.
+Wir informieren Sie gerne über die Leichtflugzeug - Pilotenlizenz SPL(A). Als LAPL(A) und PPL(A) Lizenzinhaber haben Sie die Möglichkeit, eine SPL(A) mit verkürztem Trainingsaufwand auf unserem Breezer zu erwerben.</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://air-munich.de/</t>
+        </is>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Nächster verfügbarer PPL Abendkurs
+    6. September 2021</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>http://www.fliegerverein.eu/abendkurs.htm</t>
+        </is>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Nächster Fluglehrerkurs
+    21. September 2021</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>http://www.fliegerverein.eu/fluglehrer.htm</t>
+        </is>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aktuell zur Corona – Pandemie:
+starten Sie jetzt Ihre Flugausbildung von zu Hause mit
+MFA Fernlehrgänge 2021 – garantiert “Viren Frei”
+buchbar als  “NUR THEORIEAUSBILDUNG”  NEU: Nahunterricht mit Video System (Zoom)
+</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://www.mfa.aero/de/</t>
+        </is>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wir sind für Sie da !  Sie erreichen uns jederzeit email:  info@mfa.aero
+Tel +49 89 642 707 61  –  Tel +49 821 747 24 60 
+– Theorieschulung über distance learning – ZFU genehmigt !
+– Praxisschulung nach dem Hygienekonzept von MFA !
+Covid-19 Antigen Schnelltests bei MFA verfügbar !
+MFA setzt HEPA Filter nach den Infektionsschutzmaßnahmen ein.
+! Starten Sie jetzt Ihre Ausbildung !
+</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://www.mfa.aero/de/</t>
+        </is>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Wollen Sie das Fliegen als Privatpilot lernen? Oder sich weiterbilden und Ihren Pilotenschein erweitern?Individuell, sicher und schnell? Sie wollen keine „Nummer" sein? Sie suchen professionelle Pilotenausbildung zum vernünftigen Preis?PPL (A) über CPL (A) bis ATPL (A)? Airline-Standards und zügige Copiloten-Ausbildung?Sie suchen eine professionelle Screningvorbereitung? Entweder auf einem FNPT II B737 700-800? Oder FNPT II SENECA III?Sie wollen sich zum Fluglehrer ausbilden lassen?Als gewerbliche Flugschule, (DE.ATO.005 (APPROVED TRAINING ORGANISATIONS), die vom Privatpiloten bis hin zum Berufspiloten mit Instrumentenflugberechtigung und Verkehrsflugzeugführer möchten wir uns kurz bei Ihnen vorstellen.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://www.flugausbildung.de/</t>
+        </is>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Erfolgreiche Absolventen unserer ATPL-Ausbildung sind nach bestandenem Screening als FO (First Officer = CoPilot) und später als Flugkapitän (PIC = pilot in command) u.a. bei folgenden Gesellschaften tätig:</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://www.flugausbildung.de/</t>
+        </is>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Seit bald 30 Jahren sind wir am Flugplatz Landshut-Ellermühle (30 Autominuten vom Frankfurter Ring ist Ihre Flugschule München), tätig und wir sind stets bemüht, erstklassigen Service mit günstigen, ehrlich kalkulierten Preisen zu verbinden. Unsere individuelle, fach- und sachkundige, sichere Pilotenausbildung ist weit über die Grenzen Deutschlands hinaus bekannt und beliebt. Alle Flugzeuge, die wir zur Schulung anbieten, sind unser Eigentum und schon deshalb von uns aufs Beste ausgerüstet und gewartet. Es stehen Ihnen derzeit 12 Flugzeuge, ein FNPT II MCC JET737 und ein FNPT II Twin Turbo mit Sichtsystem zur Verfügung.Professionelle Ausbildungskonzepte verbunden mit persönlicher Betreuung und individueller Zeitplanung erlauben es Ihnen vom PPL(A) bis zum ATPL(A) neben Ihrer Arbeit oder Ihrem Studium die Ausbildung bei uns zu absolvieren.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://www.flugausbildung.de/</t>
+        </is>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Start your Flight Training NOW and be ready for Take Off when the post-COVID-19 Aviation-Boom Sets in!
+Thinking about becoming an airline pilot and getting your Airline Transport Pilot License?
+Get on your career track with us:
+Request free information material now!
+Apply now and be part of our next ‘Pilot Casting Day’! Upcoming Pilot Casting Days:
+19th June 2021
+24th July 2021</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://www.eaa.aero/en/</t>
+        </is>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Current Course Schedules
+Here are the upcoming dates for our integrated Airline Transport Pilot License classes that are now ready for boarding!
+12th July 2021
+13th September 2021
+15th November 2021</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://www.eaa.aero/en/</t>
+        </is>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 8:26</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Bugfixed Scraper. Added user. Improved user management.
</commit_message>
<xml_diff>
--- a/app/PickleJar/AllTimePickle.xlsx
+++ b/app/PickleJar/AllTimePickle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,23 +476,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FMV unterzeichnet Vertrag für neues Trainingsflugzeug</t>
+          <t>Flug AF447</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Grob G 120TP für Schweden</t>
+          <t>Air France und Airbus auf Anklagebank</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Die schwedische Beschaffungsbehörde FMV hat mit Grob Aircraft SE einen...</t>
+          <t>PARIS - Rund zwölf Jahre nach dem Absturz einer Air-France-Maschine mit 228 Toten sollen der Flugzeugbauer Airbus und die Fluggesellschaft Air France auf die Anklagebank. Das Pariser Berufungsgericht ordnete am Mittwoch einen Prozess wegen fahrlässiger Tötung an, wie das Gericht in Paris bestätigte.»</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.flugrevue.de/militaer/fmv-unterzeichnet-vertrag-fuer-neues-trainingsflugzeug-grob-g-120tp-fuer-schweden/</t>
+          <t>www.aero.de/news-39619/Air-France-und-Airbus-auf-Anklagebank.html</t>
         </is>
       </c>
       <c r="F2" t="b">
@@ -500,7 +499,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2021.5.13 - 10:18</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -511,22 +510,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>„Ehe unter Verzweifelten“</t>
+          <t>Konzernkreise</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Lilium will Piloten bei Lufthansa ausbilden</t>
+          <t>Airbus traut A320neo wieder eine "Ü50"-Rate zu</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Die infolge der Corona-Krise angeschlagene Lufthansa Aviation Training...</t>
+          <t>HAMBURG - Airbus bereitet wichtige Programmpartner auf weitere Hochlaufetappen in der Produktion der A320neo-Baureihe im nächsten Jahr vor. Die Nachfrage von Airlines und Leasingfirmen nach effizienten Kurzstreckenjets kehrt schneller als erwartet zurück, Vorkrisen-Werte rücken 2022 wieder in Sichtweite.»</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.flugrevue.de/job/lilium-pilotenausbildung-bei-lufthansa/</t>
+          <t>www.aero.de/news-39610/Airbus-traut-der-A320neo-wieder-eine-Ue50-Rate-zu.html</t>
         </is>
       </c>
       <c r="F3" t="b">
@@ -534,7 +533,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2021.5.13 - 10:18</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -545,27 +544,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Unsere Breezer B400-6  ist angekommen</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>Triebwerksengpässe</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Wie Airbus 2022 neue "Glider" vermeiden will</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Eingetroffen! Für unsere Schulungen und Ausbildungen wurde die Breezer B400-6 Mitte April geliefert.
-...</t>
+          <t>HAMBURG - Vor der Krise konnten Triebwerkshersteller kaum mit der Nachfrage Schritt halten. Beim Wiederanfahren der A320neo-Produktion will Airbus Lieferstopps verhindern - der Hersteller stellt CFM und Pratt &amp; Whitney hinter den Kulissen auf steil anziehende Produktionsraten ab 2022 ein.»</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.flighttraining-service.de//aktuelles/blog/82-neue-breezer-b400-6</t>
+          <t>www.aero.de/news-39545/Wie-Airbus-2022-neue-Gilder-verhindern-will.html</t>
         </is>
       </c>
       <c r="F4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:28</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -576,27 +578,31 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neuer Sportgeräteführer (UL) Lehrgang </t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+          <t>Luftwaffe-Simulator in Nörvenich</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Eurofighter-Pilotin für 20 Minuten</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>UL Piloten Lehrgang April 2021! Neuer Sportgeräteführer (UL) Lehrgang
-...</t>
+          <t xml:space="preserve">
+Wie fliegt sich ein Eurofighter? Die Flug-Revue-Redakteurin Ulrike Ebner...</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.flighttraining-service.de//aktuelles/blog/90-neue-breezer-b400-9</t>
+          <t>https://www.flugrevue.de/militaer/eurofighter-pilotin-fuer-20-minuten/</t>
         </is>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:28</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -607,27 +613,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Umschulung auf UL Lizenz</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t xml:space="preserve">
+Lufthansa Group und BASF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Sharkskin-Technologie geht in Serie</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Umschulung von LAPL (SEP) auf UL-Lizenz Sportgeräteführer! Matthias absolviert seine Umschulung
-...</t>
+          <t>Lufthansa Cargo stattet ab 2022 alle Boeing-777-Frachter mit "AeroSHARK"...</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.flighttraining-service.de//aktuelles/blog/91-neue-breezer-b400-10</t>
+          <t>https://www.flugrevue.de/flugzeugbau/lufthansa-group-und-basf-sharkskin-technologie-geht-in-serie/</t>
         </is>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:28</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -638,22 +649,30 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>["[' ETC Announces Results of the Annual Meeting of Shareholders’ Vote', "]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>„Ehe unter Verzweifelten“</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Lilium will Piloten bei Lufthansa ausbilden</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Die infolge der Corona-Krise angeschlagene Lufthansa Aviation Training...</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-announces-results-of-the-annual-meeting-of-shareholders-vote/</t>
+          <t>https://www.flugrevue.de/job/lilium-pilotenausbildung-bei-lufthansa/</t>
         </is>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -664,22 +683,30 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>["[' -ETC Simulation Awarded Multiple Contracts for their Advanced Disaster Management Simulator (ADMS™) Totaling $2.8 Million', "]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+          <t>Nachhaltigkeit</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Flughafen München gibt Tanklager für Biokerosin frei</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>MÜNCHEN - Ab 1. Juni 2021 wird für die Betankung von Flugzeugen am Münchner Flughafen auch "grünes Kerosin" zur Verfügung stehen. Nach technischer Prüfung hat das Lufthansa-Drehkreuz sein Tanklager für klimafreundliche Flugtreibstoffe geöffnet. Die sollen in Zukunft häufiger in die Tanks fließen.»</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
+          <t>www.aero.de/news-39622/Flughafen-Muenchen-gibt-Tanklager-fuer-Biokerosin-frei.html</t>
         </is>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -690,22 +717,30 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>["[' - ETC Sterilizers Awarded Multiple Contracts for EO Vacuum Chambers and Control Upgrades Totaling $3.1 Million', "]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+          <t>"Ketchupflaschen-Effekt"</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Eurowings: Flüge innerhalb von Stunden ausverkauft</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FRANKFURT - Die deutsche Impfkampagne nimmt Fahrt auf. Flugbuchungen ziehen parallel dazu deutlich an - die Lufthansa-Tochter Eurowings schiebt für die Sommerferien Hunderte Flüge nach. Nach einem Strohfeuer über Ostern fasst auch der Veranstalter Tui deutlich mehr Vertrauen in eine planbare Nachfrage.»</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
+          <t>www.aero.de/news-39615/Eurowings-Fluege-innerhalb-von-Stunden-ausverkauft.html</t>
         </is>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -716,22 +751,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Neuer Geschäftsreisejet enthüllt</t>
+          <t>Gebührenanhebung</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Falcon 10X – Dassault will an die Spitze</t>
+          <t>Flughafen Frankfurt wird für Airlines teurer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dassault Aviation stellte am Donnerstagabend seine Falcon 10X vor, einen...</t>
+          <t>FRANKFURT - Fraport wird wegen der Corona-Krise voraussichtlich mehr als die bis Ende dieses Jahres angepeilten 4.000 Arbeitsplätze abbauen. Der Frankfurter Flughafenbetreiber stellt Airlines zudem auf steigende Gebühren am Drehkreuz ein - und risikiert einen weiteren Clinch mit Lufthansa.»</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.flugrevue.de/zivil/neuer-geschaeftsreisejet-enthuellt-falcon-10x-dassault-will-an-die-spitze/</t>
+          <t>www.aero.de/news-39613/Flughafen-Frankfurt-wird-fuer-Airlines-teurer.html</t>
         </is>
       </c>
       <c r="F10" t="b">
@@ -739,7 +774,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -750,22 +785,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lockerungen</t>
+          <t>Einigung</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Neue bundesweite Einreise-Regeln</t>
+          <t>Lufthansa übernimmt weiter Zubringerflüge für Condor</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>BERLIN - Für Urlaubsrückkehrer und andere Einreisende nach Deutschland gelten von diesem Donnerstag an bundesweit einheitliche Corona-Regeln. Für vollständig Geimpfte und Genesene fallen Vorgaben zu Quarantäne und Test-Erfordernissen weg - außer, man kommt aus einem Gebiet mit neuen, ansteckenderen Virusvarianten.»</t>
+          <t>FRANKFURT - Die beiden vom Staat geretteten Fluggesellschaften Lufthansa und Condor haben ihren Streit um Zubringerflüge vorerst auf Eis gelegt. Die beiden Unternehmen verlängerten ihre langjährige Vereinbarung, die Lufthansa im vergangenen Herbst aus Konkurrenzgründen bereits gekündigt hatte.»</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39628/Neue-bundesweite-Einreise-Regeln.html</t>
+          <t>www.aero.de/news-39606/Lufthansa-uebernimmt-weiter-Zubringerfluege-fuer-Condor.html</t>
         </is>
       </c>
       <c r="F11" t="b">
@@ -773,7 +808,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -784,22 +819,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Konzernkreise</t>
+          <t>Kreise</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Airbus traut A320neo wieder eine "Ü50"-Rate zu</t>
+          <t>Lufthansa peilt Kapitalerhöhung von drei Milliarden Euro an</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>HAMBURG - Airbus bereitet wichtige Programmpartner auf weitere Hochlaufetappen in der Produktion der A320neo-Baureihe im nächsten Jahr vor. Die Nachfrage von Airlines und Leasingfirmen nach effizienten Kurzstreckenjets kehrt schneller als erwartet zurück, Vorkrisen-Werte rücken 2022 wieder in Sichtweite.»</t>
+          <t>NEW YORK - Die Lufthansa peilt Kreisen zufolge eine Kapitalerhöhung von drei Milliarden Euro an. Zeitpunkt und Höhe seien abhängig von den Marktbedingungen, berichtete die Nachrichtenagentur Bloomberg am Montag unter Berufung auf mit der Angelegenheit vertraute Personen.»</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39610/Airbus-traut-der-A320neo-wieder-eine-Ue50-Rate-zu.html</t>
+          <t>www.aero.de/news-39601/Lufthansa-peilt-Kapitalerhoehung-von-drei-Milliarden-Euro-an.html</t>
         </is>
       </c>
       <c r="F12" t="b">
@@ -807,7 +842,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -818,22 +853,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kreise</t>
+          <t>Airlines</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Lufthansa peilt Kapitalerhöhung von drei Milliarden Euro an</t>
+          <t>Swiss droht Mindestlohn-Ärger in Genf</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>NEW YORK - Die Lufthansa peilt Kreisen zufolge eine Kapitalerhöhung von drei Milliarden Euro an. Zeitpunkt und Höhe seien abhängig von den Marktbedingungen, berichtete die Nachrichtenagentur Bloomberg am Montag unter Berufung auf mit der Angelegenheit vertraute Personen.»</t>
+          <t>GENF - Swiss gibt in der Krise jeden fünften Arbeitsplatz verloren. Vorstandschef Dieter Vranckx trimmt die Lufthansa-Tochter für eine geringere Nachfrage. Die ohnehin heiklen Verhandlungen über den Personalabbau werden von einem drohenen Tarifstreit in Genf erschwert - in der Westschweiz muss Swiss Flugbegleitern künftig deutlich mehr Gehalt zahlen.»</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39601/Lufthansa-peilt-Kapitalerhoehung-von-drei-Milliarden-Euro-an.html</t>
+          <t>www.aero.de/news-39595/Swiss-droht-Mindestlohn-Aerger-in-Genf.html</t>
         </is>
       </c>
       <c r="F13" t="b">
@@ -841,7 +876,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:39</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -852,18 +887,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Virtuelles #UnternehmenFrühstück 8vor8</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
+          <t>Pandemie</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Lufthansa fliegt über Dubai nach Indien</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Das nächste virtuelle #UnternehmenFrühstüc­k 8vor 8 findet am Mittwoch, 26. Mai, 7.52 bis 8.51 Uhr, statt und widmet sich dem Thema Networking. Mit ihrem neuen Veranstaltungsformat wollen die Industrie- und Handelskammer (IHK) Bonn/Rhein-Sieg, die Wirtschaftsförderung­en des Rhein-Sieg-Kreises und der Bundesstadt Bonn sowie die Kreishandwerkerschaf­t Bonn...</t>
+          <t>FRANKFURT - Die Lufthansa-Linien nach Indien legen vorerst einen technischen Stopp in Dubai ein. Die Airline will durch den Umweg ihre Mitarbeiter vor Infektionen mit dem Coronavirus schützen, das sich rasant im Land ausbreitet. Im Gegensatz zu anderen Airlines hält Lufthansa an ihren Linien nach Indien fest.»</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>www.pressebox.de/pressemitteilung/ihk-bonnrhein-sieg/Virtuelles-UnternehmenFruehstueck-8vor8/boxid/1058986</t>
+          <t>www.aero.de/news-39581/Lufthansa-fliegt-ueber-Dubai-nach-Indien.html</t>
         </is>
       </c>
       <c r="F14" t="b">
@@ -871,7 +910,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2021.5.14 - 10:03</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -882,26 +921,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Noch mehr Spaß an der Kurve!</t>
+          <t>["[' ETC Announces Results of the Annual Meeting of Shareholders’ Vote', "]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Im vergangenen Spätherbst führte Wunderlich das erste Fahrdynamik Training unter dem Motto „Spaß an der Kurve“ durch. Die Teilnehmerzahl war auf acht begrenzt, was für die Qualität des Trainings sprach und die Veranstaltung war im Nu ausgebucht, was für das überzeugende Konzept von „Spaß-an-der-Kurve“ sprach.</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>www.pressebox.de/pressemitteilung/wunderlich-gmbh/Noch-mehr-Spass-an-der-Kurve/boxid/1058973</t>
+          <t>https://www.etcusa.com/etc-announces-results-of-the-annual-meeting-of-shareholders-vote/</t>
         </is>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2021.5.14 - 10:03</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -912,26 +947,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Günstige Preise und seriöse Arbeitsweise – Türöffnungen und Service rund ums Schloss in München</t>
+          <t>["[' -ETC Simulation Awarded Multiple Contracts for their Advanced Disaster Management Simulator (ADMS™) Totaling $2.8 Million', "]</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Wer wo auch immer in München lebt, in der Altstadt, in einem der vielen Stadtbezirke oder auch im Umfeld der Stadt, braucht hin und wieder die Dienste eines Schlüsselservice. Vielleicht hat man den Schlüssel verloren, der Schlüssel ist im Schloss abgebrochen und es ist schnelle Hilfe nötig durch den Notfall Schlüsseldienst. Das muss auch nicht zwingend...</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>www.pressebox.de/pressemitteilung/komi-services-gmbh/Guenstige-Preise-und-serioese-Arbeitsweise-Tueroeffnungen-und-Service-rund-ums-Schloss-in-Muenchen/boxid/1059050</t>
+          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
         </is>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2021.5.14 - 18:03</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -942,30 +973,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kanzlerkandidatin der Grünen</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Baerbock will Kurzstreckenflüge abschaffen</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>BERLIN - Nach SPD-Kanzlerkandidat Olaf Scholz hat auch Grünen-Kandidatin Annalena Baerbock angekündigt, Flugreisen im Fall einer Regierungsübernahme unattraktiver machen zu wollen. Im Interview mit der "Bild am Sonntag" machte sie deutlich, dass sie perspektivisch für die Abschaffung von Kurzstreckenflügen ist.»</t>
-        </is>
-      </c>
+          <t>["[' - ETC Sterilizers Awarded Multiple Contracts for EO Vacuum Chambers and Control Upgrades Totaling $3.1 Million', "]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39649/Baerbock-will-Kurzstreckenfluege-abschaffen.html</t>
+          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
         </is>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -976,19 +999,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Italien Fliegertouren 2021</t>
+          <t>Unsere Breezer B400-6  ist angekommen</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Wir möchten nach der coronabedingten Pause nun endlich wieder mit Euch zu unseren wunderschönen und außergewöhnlichen Fliegertouren nach Italien abheben.
-Wir freuen uns sehr auf Eure Teilnahme und gemeinsame Flüge nach Italien, sowie wunderschöne Aufenthalte an den Destinationen!</t>
+          <t>Eingetroffen! Für unsere Schulungen und Ausbildungen wurde die Breezer B400-6 Mitte April geliefert.
+...</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://air-munich.de/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/82-neue-breezer-b400-6</t>
         </is>
       </c>
       <c r="F18" t="b">
@@ -996,7 +1019,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1007,18 +1030,19 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AZF Sprechfunkzeugnis</t>
+          <t xml:space="preserve">Neuer Sportgeräteführer (UL) Lehrgang </t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Am 06. und 07. März findet der nächste Kurs für das AZF Sprechfunkzeugnis statt. Für weitere Infos und Anmeldungen bitte eine Email an: office@air-munich.de</t>
+          <t>UL Piloten Lehrgang April 2021! Neuer Sportgeräteführer (UL) Lehrgang
+...</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://air-munich.de/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/90-neue-breezer-b400-9</t>
         </is>
       </c>
       <c r="F19" t="b">
@@ -1026,7 +1050,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1037,19 +1061,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Breezer B400-6</t>
+          <t>Umschulung auf UL Lizenz</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Unser Breezer B400-6 wurde im Breezer Werk in Bredstedt (Schleswig-Holstein) auf 600kg MTOM aufgerüstet, sowie mit einer elektrischen Trimmung ausgestattet.
-Wir informieren Sie gerne über die Leichtflugzeug - Pilotenlizenz SPL(A). Als LAPL(A) und PPL(A) Lizenzinhaber haben Sie die Möglichkeit, eine SPL(A) mit verkürztem Trainingsaufwand auf unserem Breezer zu erwerben.</t>
+          <t>Umschulung von LAPL (SEP) auf UL-Lizenz Sportgeräteführer! Matthias absolviert seine Umschulung
+...</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://air-munich.de/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/91-neue-breezer-b400-10</t>
         </is>
       </c>
       <c r="F20" t="b">
@@ -1057,7 +1081,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.13 - 17:36</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -1068,23 +1092,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Nächster verfügbarer PPL Abendkurs
-    6. September 2021</t>
+          <t>Noch mehr Spaß an der Kurve!</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Im vergangenen Spätherbst führte Wunderlich das erste Fahrdynamik Training unter dem Motto „Spaß an der Kurve“ durch. Die Teilnehmerzahl war auf acht begrenzt, was für die Qualität des Trainings sprach und die Veranstaltung war im Nu ausgebucht, was für das überzeugende Konzept von „Spaß-an-der-Kurve“ sprach.</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>http://www.fliegerverein.eu/abendkurs.htm</t>
+          <t>www.pressebox.de/pressemitteilung/wunderlich-gmbh/Noch-mehr-Spass-an-der-Kurve/boxid/1058973</t>
         </is>
       </c>
       <c r="F21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 10:03</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1095,23 +1122,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nächster Fluglehrerkurs
-    21. September 2021</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+          <t>Neue FAL in Toulouse</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Airbus schafft in Hamburg Platz für die A321XLR</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>HAMBURG - Der Airbus-Verkaufsschlager A321neo soll von Ende 2022 an auch am Firmensitz im südfranzösischen Toulouse zusammengebaut werden. Airbus rechnet wieder mit steigender Nachfrage im Brot-und-Butter-Programm. Das ist nicht der einzige Grund für die Einrichtung der neuen Linie.»</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>http://www.fliegerverein.eu/fluglehrer.htm</t>
+          <t>www.aero.de/news-39633/Airbus-schafft-in-Hamburg-Platz-fuer-die-A321XLR.html</t>
         </is>
       </c>
       <c r="F22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 7:33</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1122,26 +1156,30 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aktuell zur Corona – Pandemie:
-starten Sie jetzt Ihre Flugausbildung von zu Hause mit
-MFA Fernlehrgänge 2021 – garantiert “Viren Frei”
-buchbar als  “NUR THEORIEAUSBILDUNG”  NEU: Nahunterricht mit Video System (Zoom)
-</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+          <t>Sicherheit</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Airlines setzen Flüge nach Tel Aviv aus</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>FRANKFURT / TEL AVIV - Die Lufthansa setzt wegen der Eskalation im Gaza-Konflikt ihre Flüge nach Tel Aviv bis mindestens diesen Freitag aus. Auch British Airlines und alle großen US-Fluggesellschaften haben wegen des neu aufgeflammten Nahost-Konflikts alle Flüge von und nach Tel Aviv annulliert.»</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.mfa.aero/de/</t>
+          <t>www.aero.de/news-39631/Lufthansa-setzt-Fluege-nach-Tel-Aviv-aus.html</t>
         </is>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 7:33</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1152,29 +1190,30 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wir sind für Sie da !  Sie erreichen uns jederzeit email:  info@mfa.aero
-Tel +49 89 642 707 61  –  Tel +49 821 747 24 60 
-– Theorieschulung über distance learning – ZFU genehmigt !
-– Praxisschulung nach dem Hygienekonzept von MFA !
-Covid-19 Antigen Schnelltests bei MFA verfügbar !
-MFA setzt HEPA Filter nach den Infektionsschutzmaßnahmen ein.
-! Starten Sie jetzt Ihre Ausbildung !
-</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+          <t>Neue FAL in Toulouse</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Airbus schafft in Hamburg Platz für die A321XLR</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>HAMBURG - Der Airbus-Verkaufsschlager A321neo soll von Ende 2022 an auch am Firmensitz im südfranzösischen Toulouse zusammengebaut werden. Airbus rechnet wieder mit steigender Nachfrage im Brot-und-Butter-Programm. Das ist jedoch nicht der einzige Grund für die Einrichtung der neuen Linie.»</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.mfa.aero/de/</t>
+          <t>www.aero.de/news-39633/Airbus-schafft-in-Hamburg-Platz-fuer-die-A321XLR.html</t>
         </is>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 8:03</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1183,24 +1222,33 @@
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Erstes Bauteil von AeroComposite geliefert</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Wollen Sie das Fliegen als Privatpilot lernen? Oder sich weiterbilden und Ihren Pilotenschein erweitern?Individuell, sicher und schnell? Sie wollen keine „Nummer" sein? Sie suchen professionelle Pilotenausbildung zum vernünftigen Preis?PPL (A) über CPL (A) bis ATPL (A)? Airline-Standards und zügige Copiloten-Ausbildung?Sie suchen eine professionelle Screningvorbereitung? Entweder auf einem FNPT II B737 700-800? Oder FNPT II SENECA III?Sie wollen sich zum Fluglehrer ausbilden lassen?Als gewerbliche Flugschule, (DE.ATO.005 (APPROVED TRAINING ORGANISATIONS), die vom Privatpiloten bis hin zum Berufspiloten mit Instrumentenflugberechtigung und Verkehrsflugzeugführer möchten wir uns kurz bei Ihnen vorstellen.</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>Russischer Kohlefaserflügel für MS-21</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Airbus arbeitet in Toulouse an einer modernisierten...</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.flugausbildung.de/</t>
+          <t>https://shop.motorpresse.de/flugrevue/abo/abo-fur-mich/?hnr=extern.verlag.flugrevue.navigation</t>
         </is>
       </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 11:03</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
@@ -1209,24 +1257,35 @@
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Testprogramm gleich bei Großübung in Alaska</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Erfolgreiche Absolventen unserer ATPL-Ausbildung sind nach bestandenem Screening als FO (First Officer = CoPilot) und später als Flugkapitän (PIC = pilot in command) u.a. bei folgenden Gesellschaften tätig:</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
+          <t xml:space="preserve">
+F-15EX fliegt bei „Northern Edge“</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Airbus arbeitet in Toulouse an einer modernisierten...</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.flugausbildung.de/</t>
+          <t>https://shop.motorpresse.de/flugrevue/abo/abo-fur-mich/?hnr=extern.verlag.flugrevue.navigation</t>
         </is>
       </c>
       <c r="F26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 11:03</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1235,24 +1294,33 @@
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Nachnutzung der A380-Anlagen</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Seit bald 30 Jahren sind wir am Flugplatz Landshut-Ellermühle (30 Autominuten vom Frankfurter Ring ist Ihre Flugschule München), tätig und wir sind stets bemüht, erstklassigen Service mit günstigen, ehrlich kalkulierten Preisen zu verbinden. Unsere individuelle, fach- und sachkundige, sichere Pilotenausbildung ist weit über die Grenzen Deutschlands hinaus bekannt und beliebt. Alle Flugzeuge, die wir zur Schulung anbieten, sind unser Eigentum und schon deshalb von uns aufs Beste ausgerüstet und gewartet. Es stehen Ihnen derzeit 12 Flugzeuge, ein FNPT II MCC JET737 und ein FNPT II Twin Turbo mit Sichtsystem zur Verfügung.Professionelle Ausbildungskonzepte verbunden mit persönlicher Betreuung und individueller Zeitplanung erlauben es Ihnen vom PPL(A) bis zum ATPL(A) neben Ihrer Arbeit oder Ihrem Studium die Ausbildung bei uns zu absolvieren.</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
+          <t>Neue A320-Montagelinie in Toulouse</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Airbus arbeitet in Toulouse an einer modernisierten...</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.flugausbildung.de/</t>
+          <t>https://shop.motorpresse.de/flugrevue/abo/abo-fur-mich/?hnr=extern.verlag.flugrevue.navigation</t>
         </is>
       </c>
       <c r="F27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 11:03</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
@@ -1261,30 +1329,32 @@
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sicherheit</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Start your Flight Training NOW and be ready for Take Off when the post-COVID-19 Aviation-Boom Sets in!
-Thinking about becoming an airline pilot and getting your Airline Transport Pilot License?
-Get on your career track with us:
-Request free information material now!
-Apply now and be part of our next ‘Pilot Casting Day’! Upcoming Pilot Casting Days:
-19th June 2021
-24th July 2021</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
+          <t>Airlines setzen Flüge nach Tel Aviv aus</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>FRANKFURT / TEL AVIV - Die Lufthansa setzt wegen der Eskalation im Gaza-Konflikt ihre Flüge nach Tel Aviv bis mindestens diesen Freitag aus. Auch British Airways, Wizz Air und alle großen US-Fluggesellschaften haben wegen des neu aufgeflammten Nahost-Konflikts alle Flüge von und nach Tel Aviv annulliert.»</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.eaa.aero/en/</t>
+          <t>www.aero.de/news-39631/Lufthansa-setzt-Fluege-nach-Tel-Aviv-aus.html</t>
         </is>
       </c>
       <c r="F28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 11:33</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1293,31 +1363,691 @@
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Sicherheit</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Current Course Schedules
-Here are the upcoming dates for our integrated Airline Transport Pilot License classes that are now ready for boarding!
-12th July 2021
-13th September 2021
-15th November 2021</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
+          <t>EASA warnt vor Flügen im israelischen Luftraum</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>TEL AVIV - Israel hat am Freitagmorgen Luftangriffe auf Hamas-Stellungen in Gaza geflogen und erstmals Bodentruppen eingesetzt. Hamas-Kämpfer feuerten erneut Raketen auf israelisches Gebiet ab. Die europäische Luftfahrtaufsicht EASA warnt vor Gefahren für den zivilen Luftverkehr in der Region.»</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.eaa.aero/en/</t>
+          <t>www.aero.de/news-39638/EASA-warnt-vor-Fluegen-im-israelischen-Luftraum.html</t>
         </is>
       </c>
       <c r="F29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2021.5.17 - 8:26</t>
+          <t>2021.5.14 - 13:03</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Schweizer Turboprop</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Pilatus liefert 1800. PC-12 aus</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Embraer hat mit der Aerodata AG aus Braunschweig einen Vertrag über den Kauf einer Praetor 600 unterzeichnet. Der Business Jet soll 2022...</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://www.aerokurier.de</t>
+        </is>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2021.5.14 - 14:33</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Schweizer Turboprop</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Pilatus liefert 1800. PC-12 aus</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Pilatus hat den 1800. PC-12 an einen Kunden übergeben. Neuer...</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://www.aerokurier.de/business-aviation/schweizer-turboprop-pilatus-liefert-1800-pc-12-aus/</t>
+        </is>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2021.5.14 - 14:33</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Sicherheit</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Lufthansa verlängert Flugstopp nach Israel</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>FRANKFURT - Angesichts des militärischen Konflikts in Israel hat die Lufthansa-Gruppe weitere Flüge in die Region gestrichen.»</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>www.aero.de/news-39641/Lufthansa-verlaengert-Flugstopp-nach-Israel.html</t>
+        </is>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2021.5.14 - 16:33</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Sikorsky and Rheinmetall continue to count on German industrial team: Reiser strengthens education and training of maintenance staff</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>January 27, 2021 Heavy-lift helicopter: Sikorsky and Rheinmetall expand German industrial partnership on CH-53K Teaming agreement renewed: Sikorsky and Rheinmetall continue to count on German industrial team Bavarian Mittelstand company Reiser strengthens education and training of maintenance staff Berlin/Düsseldorf/Berg, January 27, 2021 – Sikorsky and the members of the German CH-53K industry team have reaffirmed […]</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/sikorsky-and-rheinmetall-continue-to-count-on-german-industrial-team-reiser-strengthens-education-and-training-of-maintenance-staff/</t>
+        </is>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Joint Press Release on Successful EASA Level D Qualification of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator at Norwegian Competence Centre Helicopter AS (NCCH)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Berg, Germany / Stavanger, Norway, October 8, 2020 Last week the first-of-its-kind H135 (EC135 T3H) full flight simulator was initially qualified as to the highest standard Level D by the responsible competent aviation authority CAA Norway. Therefore the simulator is now available for training under European Aviation Safety Agency (EASA) regulations. This simulator is a […]</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/joint-press-release-on-successful-easa-level-d-qualification-of-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulator-at-norwegian-competence-centre-helicopter-as-ncch/</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Airbus Defence and Space selects Reiser Simulation and Training for the Provision of Eurofighter Synthetic Training System Cockpits Replacement</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Berg, Germany, October 12, 2020 – Today’s aviation training requirements are changing, especially in the field of synthetic pilot training. The German MOD has contracted Airbus Defence and Space to extend the Eurofighter/Typhoon Pilot Synthetic Training System (PSTS) at the Main Operating Base (MOB) in Laage and introduce state-of-the-art simulator cockpits at all Eurofighter MOBs […]</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/airbus-defence-and-space-selects-reiser-simulation-and-training-for-the-provision-of-eurofighter-synthetic-training-system-cockpits-replacement/</t>
+        </is>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2021-02 RHT/UWETS Asia</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>We are proud to announce a repeat order for a combined Rescue Hoist and Under Water Escape Training System. The order was placed by the South-East Asian customer who ordered the same system in October last year. We would like to thank them for their great confidence after the short period of cooperation.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2021-02 Normobaric Hypoxia Acceptance</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>AMST successfully handed over two Reduced Oxygen Breathing Devices (ROBDs) for normobaric hypoxia training to two of its AIRFOX customers. The devices are part of upgrades to existing AIRFOX ASD and AIRFOX DISO systems.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2021-02-normobaric-hypoxia-acceptance-162/</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2020-12 Charity Donation</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Already in early autumn, the staff at our headquarters in Ranshofen decided to donate to a charitable cause instead of having a Christmas party. It was very important to the employees to support people in need living around the company location in these difficult times. The amount of 4350 Euros was given to two charities: The Children’s Cancer Help Organisation for Upper Austria and Braunau Life Aid.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2020-11 Engl Flightteam Cooperation</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Engl Flightteam, a flight training provider, signed a partnership agreement with AMST in October 2020. The cooperation focusses on Spatial Disorientation training on our AIRFOX ASD and Multi Crew Coordination (MCC) training on our newly qualified AIRFOX UPRT simulator. We wish all trainees a great time at AMST and an excellent experience with our simulation equipment.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2020-11-18 COVID Situation Update</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dear Business Partners and Colleagues!
+Austria’s government implemented a hard lockdown starting 17 November 2020 to curb COVID infection rates. AMST has already demonstrated during the first lockdown in Spring that it has the necessary structures, tools and – most importantly – the determination to ensure continuity and success of its business. </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2020-11-18-covid-situation-update-156/</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2020-11 RHT/UWETS Asia</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>AMST’s leading role for Rescue Hoist Training was underlined by a second contract for a Rescue Hoist Trainer (RHT) within the year 2020 from a South-East Asian Training Organisation. The contract also includes a complete Underwater Egress Training System (UWETS) with parachute training equipment.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2020-11-rhtuwets-asia-155/</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2021-02 FFS UPRT Upgrade</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>We are pleased to announce an additional contract award placed in January 2021. This extensive software upgrade, including UPRT to an in-service FFS, will be implemented and completed in just 12 weeks.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2021-02-ffs-uprt-upgrade-164/</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2020-11 AMST at GATS-V 2020</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>AMST participates in the Global Airline Training &amp; Simulation (GATS) Virtual Conference and Tradeshow taking place from 10-12 Nov. 2020. You can visit our virtual booth at www.gats-event.com. We are looking forward to present to you our ground-breaking solutions for best quality pilot training.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.athttps://www.gats-event.com</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2020-07 AMST now on YouTube</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>AMST is now on YouTube with videos in HD and playlists for our business units. Enjoy, share and subscribe to our channel to stay updated!</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.athttps://www.youtube.com/channel/UCOKLkJRlI2MLPagBC-3gCIg/playlists</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2020-06 AIRFOX UPRT Qualification</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>AMST is delighted to announce the qualification of our intermediate training device as a Generic Multi Engine Turbofan Aeroplane FNPT II MCC by EASA.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-06-airfox-uprt-qualification-147/</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2020-04-21 CEO Message</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dear Customers, Partners, Suppliers and Colleagues!
+As we are already in the 6th week under COVID restrictions, I would like to say a big „Thank You!“ to all of you for taking the highest effort to run a more or less regular business together! </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-04-21-ceo-message-143/</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2020-03-17 Corona Virus Situation</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A message from the AMST Group's CEO regarding the current Corona virus situation. </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-03-17-corona-virus-situation-140/</t>
+        </is>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2019-10 AIRFOX FFS Level D Qualification</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AMST is delighted to announce the qualification of our first A320 NEO Full Flight Simulator (White Tail) to an EASA CS-FSTD(A)-Issue 2 Level D standard. This Full Flight Simulator was designed and built by AMST Aviation BV, at our facility in the Netherlands (close to Schiphol Airport). </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2019-10-airfox-ffs-level-d-qualification-124/</t>
+        </is>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2019-10 EATS Berlin</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>AMST-Aviation will participate in the European Airline Training Symposium (EATS), which takes place from 29-30 October 2019 in Berlin. Visit us at our booth 114 to discuss with our CEO, CTO and other subject matter experts the exciting solutions AMST-Aviation offers for your training needs.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2019-09 APATS Singapore</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>AMST-Aviation will participate in the Asia Pacific Airline Training Summit (APATS), which takes place from 3-4 September 2019 at the Sands Expo Convention centre in Singapore. Visit us at our booth 201 to discuss with our CEO, CTO and other subject matter experts the exciting solutions AMST-Aviation offers for your training needs.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2019-05 WATS Orlando</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>AMST will participate at WATS 2019 in Orlando, USA. We are looking forward to meeting with worldwide leading airlines and training organisations. If you are interested in talking to us at the conference, please contact us via e-mail office@amst-aviation.com or use the conference app.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2021.5.17 - 15:29</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Bugfixed REISER; changed offline testing scripts
</commit_message>
<xml_diff>
--- a/app/PickleJar/AllTimePickle.xlsx
+++ b/app/PickleJar/AllTimePickle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2049,6 +2049,439 @@
       </c>
       <c r="H51" t="inlineStr"/>
     </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Die Bell 525 hat einen ersten Flug mit SAF absolviert                            
+premium</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Nachdem Bell Textron seit März 2021 nachhaltig produzierten Treibstoff (SAF) für seine eigene Vorführ- und Trainingsflotte nutzt, hat der Hersteller nun bekanntgegeben, […]</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>https://aerobuzz.de/helikopter/die-bell-525-hat-einen-ersten-flug-mit-saf-absolviert/</t>
+        </is>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>["[' - ETC Awarded Contract from the University of North Dakota’s John D. Odegard School of Aerospace Sciences', "]</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>https://www.etcusa.com/etc-awarded-contract-from-the-university-of-north-dakotas-john-d-odegard-school-of-aerospace-sciences/</t>
+        </is>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>["[' - ETC Announces Notice of Annual Meeting of Shareholders', "]</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>https://www.etcusa.com/etc-announces-notice-of-annual-meeting-of-shareholders-2/</t>
+        </is>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>["[' ETC Announces Fiscal 2022 Second Quarter Results', "]</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>https://www.etcusa.com/etc-announces-fiscal-2022-second-quarter-results/</t>
+        </is>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Reiser Simulation and Training teams up with RS Flight Systems to provide new product line on FNPTs and FTDs to the helicpoter training market</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Berg, Germany, 30.09.2021 Reiser Simulation and Training GmbH (RST) has teamed up with RS Flight Systems GmbH (RSFS) to provide innovative and cost-effective FNPT and FTD products to the market. The new product line called “F-light line” for “Flightsimulator light” will feature the well-proven Level D capable flight model together with the Helionix® avionics replica, […]</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-teams-up-with-rs-flight-systems-to-provide-new-product-line-on-fnpts-andftds-to-the-helicpoter-training-market/</t>
+        </is>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Reiser Simulation and Training GmbH to Expand Helicopter Full Flight Simulator Portfolio</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Berg, Germany, September 16, 2021 Reiser Simulation and Training GmbH (RST) expands its portfolio of innovative flight training solutions. The German simulator manufacturer is proud of having welcomed Swiss Air-Rescue (Rega) and Leonardo Helicopters to its headquarters for the signing of their latest contract. RST has been awarded a contract from Rega for the provision […]</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-to-expand-helicopter-full-flight-simulator-portfolio/</t>
+        </is>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Successful EASA Level D Qualification&lt;br&gt;of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator&lt;br&gt;at Lufthansa Aviation Training GmbH (LAT)</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Berg / Frankfurt a. Main / Germany, May 31, 2021 RST’s newest Airbus H135 full flight simulator was initially qualified to the highest standard Level D by the German Federal Aviation Office (Luftfahrt-Bundesamt / LBA) according to European Aviation Safety Agency (EASA) regulations. The most modern FFS helicopter type H135 is thus ready for training […]</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/successful-easa-level-d-qualificationof-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulatorat-lufthansa-aviation-training-gmbh-lat/</t>
+        </is>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+RHT/UWETS Asia Repeat Order </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+				News				
+2021-02-15 
+</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			We are proud to announce a repeat order for a combined Rescue Hoist and Under Water Escape Training System. The...		</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-aerospace-medicine/rht-uwets-asia-repeat-order/</t>
+        </is>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Normobaric Hypoxia Acceptance </t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+				News				
+2021-02-09 
+</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			AMST successfully handed over two Reduced Oxygen Breathing Devices (ROBDs) for normobaric hypoxia training to two of its AIRFOX customers....		</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-aerospace-medicine/normobaric-hypoxia-acceptance/</t>
+        </is>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Charity Donation </t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+				News				
+2020-12-16 
+</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			Already in early autumn, the staff at our headquarters in Ranshofen decided to donate to a charitable cause instead of...		</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-aerospace-medicine/charity-donation/</t>
+        </is>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+AMST at WATS 2021 </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+				News				
+2021-06-11 
+</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			AMST is participating in the World Aviation Training Summit (WATS) taking place on 15 and 16 of June 2021 in Orlando Florida. Join us at our booth #223 to have...		</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-civil-aviation/amst-at-wats-2021/</t>
+        </is>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+FFS UPRT Upgrade </t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+				News				
+2021-02-15 
+</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			Upset Prevention and Recovery Training (UPRT) remains a crucial topic in our industry. AMST has developed and delivered a range of solutions to this demanding requirement. We have applied almost...		</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-civil-aviation/ffs-uprt-upgrade/</t>
+        </is>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Engl Flightteam Cooperation </t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+				News				
+2020-11-20 
+</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			Engl Flightteam, a flight training provider, signed a partnership agreement with AMST in October 2020. The cooperation focusses on Spatial Disorientation training on our AIRFOX ASD and Multi Crew Coordination...		</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-aerospace-medicine/engl-flightteam-cooperation/</t>
+        </is>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2021.11.25 - 15:58</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
activated mail-sending of TestMail again; repaired changed Pressebox; added SingularityHub.com
</commit_message>
<xml_diff>
--- a/app/PickleJar/AllTimePickle.xlsx
+++ b/app/PickleJar/AllTimePickle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,30 +476,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Flug AF447</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Air France und Airbus auf Anklagebank</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>PARIS - Rund zwölf Jahre nach dem Absturz einer Air-France-Maschine mit 228 Toten sollen der Flugzeugbauer Airbus und die Fluggesellschaft Air France auf die Anklagebank. Das Pariser Berufungsgericht ordnete am Mittwoch einen Prozess wegen fahrlässiger Tötung an, wie das Gericht in Paris bestätigte.»</t>
-        </is>
-      </c>
+          <t>["[' ETC Announces Results of the Annual Meeting of Shareholders’ Vote', "]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39619/Air-France-und-Airbus-auf-Anklagebank.html</t>
+          <t>https://www.etcusa.com/etc-announces-results-of-the-annual-meeting-of-shareholders-vote/</t>
         </is>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -510,30 +502,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Konzernkreise</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Airbus traut A320neo wieder eine "Ü50"-Rate zu</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>HAMBURG - Airbus bereitet wichtige Programmpartner auf weitere Hochlaufetappen in der Produktion der A320neo-Baureihe im nächsten Jahr vor. Die Nachfrage von Airlines und Leasingfirmen nach effizienten Kurzstreckenjets kehrt schneller als erwartet zurück, Vorkrisen-Werte rücken 2022 wieder in Sichtweite.»</t>
-        </is>
-      </c>
+          <t>["[' -ETC Simulation Awarded Multiple Contracts for their Advanced Disaster Management Simulator (ADMS™) Totaling $2.8 Million', "]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39610/Airbus-traut-der-A320neo-wieder-eine-Ue50-Rate-zu.html</t>
+          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
         </is>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -544,30 +528,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Triebwerksengpässe</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Wie Airbus 2022 neue "Glider" vermeiden will</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>HAMBURG - Vor der Krise konnten Triebwerkshersteller kaum mit der Nachfrage Schritt halten. Beim Wiederanfahren der A320neo-Produktion will Airbus Lieferstopps verhindern - der Hersteller stellt CFM und Pratt &amp; Whitney hinter den Kulissen auf steil anziehende Produktionsraten ab 2022 ein.»</t>
-        </is>
-      </c>
+          <t>["[' - ETC Sterilizers Awarded Multiple Contracts for EO Vacuum Chambers and Control Upgrades Totaling $3.1 Million', "]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39545/Wie-Airbus-2022-neue-Gilder-verhindern-will.html</t>
+          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
         </is>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -578,31 +554,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Luftwaffe-Simulator in Nörvenich</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Eurofighter-Pilotin für 20 Minuten</t>
-        </is>
-      </c>
+          <t>Unsere Breezer B400-6  ist angekommen</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Wie fliegt sich ein Eurofighter? Die Flug-Revue-Redakteurin Ulrike Ebner...</t>
+          <t>Eingetroffen! Für unsere Schulungen und Ausbildungen wurde die Breezer B400-6 Mitte April geliefert.
+...</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.flugrevue.de/militaer/eurofighter-pilotin-fuer-20-minuten/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/82-neue-breezer-b400-6</t>
         </is>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -613,32 +585,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Lufthansa Group und BASF</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Sharkskin-Technologie geht in Serie</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Neuer Sportgeräteführer (UL) Lehrgang </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lufthansa Cargo stattet ab 2022 alle Boeing-777-Frachter mit "AeroSHARK"...</t>
+          <t>UL Piloten Lehrgang April 2021! Neuer Sportgeräteführer (UL) Lehrgang
+...</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.flugrevue.de/flugzeugbau/lufthansa-group-und-basf-sharkskin-technologie-geht-in-serie/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/90-neue-breezer-b400-9</t>
         </is>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -649,30 +616,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>„Ehe unter Verzweifelten“</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Lilium will Piloten bei Lufthansa ausbilden</t>
-        </is>
-      </c>
+          <t>Umschulung auf UL Lizenz</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Die infolge der Corona-Krise angeschlagene Lufthansa Aviation Training...</t>
+          <t>Umschulung von LAPL (SEP) auf UL-Lizenz Sportgeräteführer! Matthias absolviert seine Umschulung
+...</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.flugrevue.de/job/lilium-pilotenausbildung-bei-lufthansa/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/91-neue-breezer-b400-10</t>
         </is>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -683,30 +647,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nachhaltigkeit</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Flughafen München gibt Tanklager für Biokerosin frei</t>
-        </is>
-      </c>
+          <t>Italien Fliegertouren 2021</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MÜNCHEN - Ab 1. Juni 2021 wird für die Betankung von Flugzeugen am Münchner Flughafen auch "grünes Kerosin" zur Verfügung stehen. Nach technischer Prüfung hat das Lufthansa-Drehkreuz sein Tanklager für klimafreundliche Flugtreibstoffe geöffnet. Die sollen in Zukunft häufiger in die Tanks fließen.»</t>
+          <t>Wir möchten nach der coronabedingten Pause nun endlich wieder mit Euch zu unseren wunderschönen und außergewöhnlichen Fliegertouren nach Italien abheben.
+Wir freuen uns sehr auf Eure Teilnahme und gemeinsame Flüge nach Italien, sowie wunderschöne Aufenthalte an den Destinationen!</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39622/Flughafen-Muenchen-gibt-Tanklager-fuer-Biokerosin-frei.html</t>
+          <t>https://air-munich.de/</t>
         </is>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -717,30 +678,26 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>"Ketchupflaschen-Effekt"</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Eurowings: Flüge innerhalb von Stunden ausverkauft</t>
-        </is>
-      </c>
+          <t>AZF Sprechfunkzeugnis</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FRANKFURT - Die deutsche Impfkampagne nimmt Fahrt auf. Flugbuchungen ziehen parallel dazu deutlich an - die Lufthansa-Tochter Eurowings schiebt für die Sommerferien Hunderte Flüge nach. Nach einem Strohfeuer über Ostern fasst auch der Veranstalter Tui deutlich mehr Vertrauen in eine planbare Nachfrage.»</t>
+          <t>Am 06. und 07. März findet der nächste Kurs für das AZF Sprechfunkzeugnis statt. Für weitere Infos und Anmeldungen bitte eine Email an: office@air-munich.de</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39615/Eurowings-Fluege-innerhalb-von-Stunden-ausverkauft.html</t>
+          <t>https://air-munich.de/</t>
         </is>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -751,30 +708,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gebührenanhebung</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Flughafen Frankfurt wird für Airlines teurer</t>
-        </is>
-      </c>
+          <t>Breezer B400-6</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>FRANKFURT - Fraport wird wegen der Corona-Krise voraussichtlich mehr als die bis Ende dieses Jahres angepeilten 4.000 Arbeitsplätze abbauen. Der Frankfurter Flughafenbetreiber stellt Airlines zudem auf steigende Gebühren am Drehkreuz ein - und risikiert einen weiteren Clinch mit Lufthansa.»</t>
+          <t>Unser Breezer B400-6 wurde im Breezer Werk in Bredstedt (Schleswig-Holstein) auf 600kg MTOM aufgerüstet, sowie mit einer elektrischen Trimmung ausgestattet.
+Wir informieren Sie gerne über die Leichtflugzeug - Pilotenlizenz SPL(A). Als LAPL(A) und PPL(A) Lizenzinhaber haben Sie die Möglichkeit, eine SPL(A) mit verkürztem Trainingsaufwand auf unserem Breezer zu erwerben.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39613/Flughafen-Frankfurt-wird-fuer-Airlines-teurer.html</t>
+          <t>https://air-munich.de/</t>
         </is>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -785,30 +739,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Einigung</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Lufthansa übernimmt weiter Zubringerflüge für Condor</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>FRANKFURT - Die beiden vom Staat geretteten Fluggesellschaften Lufthansa und Condor haben ihren Streit um Zubringerflüge vorerst auf Eis gelegt. Die beiden Unternehmen verlängerten ihre langjährige Vereinbarung, die Lufthansa im vergangenen Herbst aus Konkurrenzgründen bereits gekündigt hatte.»</t>
-        </is>
-      </c>
+          <t>Nächster verfügbarer PPL Abendkurs
+    6. September 2021</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39606/Lufthansa-uebernimmt-weiter-Zubringerfluege-fuer-Condor.html</t>
+          <t>http://www.fliegerverein.eu/abendkurs.htm</t>
         </is>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -819,30 +766,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Kreise</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Lufthansa peilt Kapitalerhöhung von drei Milliarden Euro an</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>NEW YORK - Die Lufthansa peilt Kreisen zufolge eine Kapitalerhöhung von drei Milliarden Euro an. Zeitpunkt und Höhe seien abhängig von den Marktbedingungen, berichtete die Nachrichtenagentur Bloomberg am Montag unter Berufung auf mit der Angelegenheit vertraute Personen.»</t>
-        </is>
-      </c>
+          <t>Nächster Fluglehrerkurs
+    21. September 2021</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39601/Lufthansa-peilt-Kapitalerhoehung-von-drei-Milliarden-Euro-an.html</t>
+          <t>http://www.fliegerverein.eu/fluglehrer.htm</t>
         </is>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -853,30 +793,26 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Airlines</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Swiss droht Mindestlohn-Ärger in Genf</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>GENF - Swiss gibt in der Krise jeden fünften Arbeitsplatz verloren. Vorstandschef Dieter Vranckx trimmt die Lufthansa-Tochter für eine geringere Nachfrage. Die ohnehin heiklen Verhandlungen über den Personalabbau werden von einem drohenen Tarifstreit in Genf erschwert - in der Westschweiz muss Swiss Flugbegleitern künftig deutlich mehr Gehalt zahlen.»</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Aktuell zur Corona – Pandemie:
+starten Sie jetzt Ihre Flugausbildung von zu Hause mit
+MFA Fernlehrgänge 2021 – garantiert “Viren Frei”
+buchbar als  “NUR THEORIEAUSBILDUNG”  NEU: Nahunterricht mit Video System (Zoom)
+</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39595/Swiss-droht-Mindestlohn-Aerger-in-Genf.html</t>
+          <t>https://www.mfa.aero/de/</t>
         </is>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -887,30 +823,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Pandemie</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Lufthansa fliegt über Dubai nach Indien</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>FRANKFURT - Die Lufthansa-Linien nach Indien legen vorerst einen technischen Stopp in Dubai ein. Die Airline will durch den Umweg ihre Mitarbeiter vor Infektionen mit dem Coronavirus schützen, das sich rasant im Land ausbreitet. Im Gegensatz zu anderen Airlines hält Lufthansa an ihren Linien nach Indien fest.»</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Wir sind für Sie da !  Sie erreichen uns jederzeit email:  info@mfa.aero
+Tel +49 89 642 707 61  –  Tel +49 821 747 24 60 
+– Theorieschulung über distance learning – ZFU genehmigt !
+– Praxisschulung nach dem Hygienekonzept von MFA !
+Covid-19 Antigen Schnelltests bei MFA verfügbar !
+MFA setzt HEPA Filter nach den Infektionsschutzmaßnahmen ein.
+! Starten Sie jetzt Ihre Ausbildung !
+</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39581/Lufthansa-fliegt-ueber-Dubai-nach-Indien.html</t>
+          <t>https://www.mfa.aero/de/</t>
         </is>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -919,16 +854,16 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>["[' ETC Announces Results of the Annual Meeting of Shareholders’ Vote', "]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Wollen Sie das Fliegen als Privatpilot lernen? Oder sich weiterbilden und Ihren Pilotenschein erweitern?Individuell, sicher und schnell? Sie wollen keine „Nummer" sein? Sie suchen professionelle Pilotenausbildung zum vernünftigen Preis?PPL (A) über CPL (A) bis ATPL (A)? Airline-Standards und zügige Copiloten-Ausbildung?Sie suchen eine professionelle Screningvorbereitung? Entweder auf einem FNPT II B737 700-800? Oder FNPT II SENECA III?Sie wollen sich zum Fluglehrer ausbilden lassen?Als gewerbliche Flugschule, (DE.ATO.005 (APPROVED TRAINING ORGANISATIONS), die vom Privatpiloten bis hin zum Berufspiloten mit Instrumentenflugberechtigung und Verkehrsflugzeugführer möchten wir uns kurz bei Ihnen vorstellen.</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-announces-results-of-the-annual-meeting-of-shareholders-vote/</t>
+          <t>https://www.flugausbildung.de/</t>
         </is>
       </c>
       <c r="F15" t="b">
@@ -936,7 +871,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -945,16 +880,16 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>["[' -ETC Simulation Awarded Multiple Contracts for their Advanced Disaster Management Simulator (ADMS™) Totaling $2.8 Million', "]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Erfolgreiche Absolventen unserer ATPL-Ausbildung sind nach bestandenem Screening als FO (First Officer = CoPilot) und später als Flugkapitän (PIC = pilot in command) u.a. bei folgenden Gesellschaften tätig:</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
+          <t>https://www.flugausbildung.de/</t>
         </is>
       </c>
       <c r="F16" t="b">
@@ -962,7 +897,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -971,16 +906,16 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>["[' - ETC Sterilizers Awarded Multiple Contracts for EO Vacuum Chambers and Control Upgrades Totaling $3.1 Million', "]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Seit bald 30 Jahren sind wir am Flugplatz Landshut-Ellermühle (30 Autominuten vom Frankfurter Ring ist Ihre Flugschule München), tätig und wir sind stets bemüht, erstklassigen Service mit günstigen, ehrlich kalkulierten Preisen zu verbinden. Unsere individuelle, fach- und sachkundige, sichere Pilotenausbildung ist weit über die Grenzen Deutschlands hinaus bekannt und beliebt. Alle Flugzeuge, die wir zur Schulung anbieten, sind unser Eigentum und schon deshalb von uns aufs Beste ausgerüstet und gewartet. Es stehen Ihnen derzeit 12 Flugzeuge, ein FNPT II MCC JET737 und ein FNPT II Twin Turbo mit Sichtsystem zur Verfügung.Professionelle Ausbildungskonzepte verbunden mit persönlicher Betreuung und individueller Zeitplanung erlauben es Ihnen vom PPL(A) bis zum ATPL(A) neben Ihrer Arbeit oder Ihrem Studium die Ausbildung bei uns zu absolvieren.</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-sterilizers-awarded-multiple-contracts-for-eo-vacuum-chambers-and-control-upgrades-totaling-3-1-million/</t>
+          <t>https://www.flugausbildung.de/</t>
         </is>
       </c>
       <c r="F17" t="b">
@@ -988,7 +923,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -997,21 +932,22 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Unsere Breezer B400-6  ist angekommen</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Eingetroffen! Für unsere Schulungen und Ausbildungen wurde die Breezer B400-6 Mitte April geliefert.
-...</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Start your Flight Training NOW and be ready for Take Off when the post-COVID-19 Aviation-Boom Sets in!
+Thinking about becoming an airline pilot and getting your Airline Transport Pilot License?
+Get on your career track with us:
+Request free information material now!
+Apply now and be part of our next ‘Pilot Casting Day’! Upcoming Pilot Casting Days:
+19th June 2021
+24th July 2021</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.flighttraining-service.de//aktuelles/blog/82-neue-breezer-b400-6</t>
+          <t>https://www.eaa.aero/en/</t>
         </is>
       </c>
       <c r="F18" t="b">
@@ -1019,7 +955,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1028,21 +964,20 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Neuer Sportgeräteführer (UL) Lehrgang </t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>UL Piloten Lehrgang April 2021! Neuer Sportgeräteführer (UL) Lehrgang
-...</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Current Course Schedules
+Here are the upcoming dates for our integrated Airline Transport Pilot License classes that are now ready for boarding!
+12th July 2021
+13th September 2021
+15th November 2021</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.flighttraining-service.de//aktuelles/blog/90-neue-breezer-b400-9</t>
+          <t>https://www.eaa.aero/en/</t>
         </is>
       </c>
       <c r="F19" t="b">
@@ -1050,7 +985,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.16 - 13:58</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1061,19 +996,18 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Umschulung auf UL Lizenz</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Umschulung von LAPL (SEP) auf UL-Lizenz Sportgeräteführer! Matthias absolviert seine Umschulung
-...</t>
-        </is>
-      </c>
+          <t>Sikorsky and Rheinmetall continue to count on German industrial team: Reiser strengthens education and training of maintenance staff</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>January 27, 2021 Heavy-lift helicopter: Sikorsky and Rheinmetall expand German industrial partnership on CH-53K Teaming agreement renewed: Sikorsky and Rheinmetall continue to count on German industrial team Bavarian Mittelstand company Reiser strengthens education and training of maintenance staff Berlin/Düsseldorf/Berg, January 27, 2021 – Sikorsky and the members of the German CH-53K industry team have reaffirmed […]</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.flighttraining-service.de//aktuelles/blog/91-neue-breezer-b400-10</t>
+          <t>https://www.reiser-st.com/sikorsky-and-rheinmetall-continue-to-count-on-german-industrial-team-reiser-strengthens-education-and-training-of-maintenance-staff/</t>
         </is>
       </c>
       <c r="F20" t="b">
@@ -1081,7 +1015,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2021.5.13 - 17:36</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -1092,26 +1026,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Noch mehr Spaß an der Kurve!</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Im vergangenen Spätherbst führte Wunderlich das erste Fahrdynamik Training unter dem Motto „Spaß an der Kurve“ durch. Die Teilnehmerzahl war auf acht begrenzt, was für die Qualität des Trainings sprach und die Veranstaltung war im Nu ausgebucht, was für das überzeugende Konzept von „Spaß-an-der-Kurve“ sprach.</t>
-        </is>
-      </c>
+          <t>Joint Press Release on Successful EASA Level D Qualification of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator at Norwegian Competence Centre Helicopter AS (NCCH)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Berg, Germany / Stavanger, Norway, October 8, 2020 Last week the first-of-its-kind H135 (EC135 T3H) full flight simulator was initially qualified as to the highest standard Level D by the responsible competent aviation authority CAA Norway. Therefore the simulator is now available for training under European Aviation Safety Agency (EASA) regulations. This simulator is a […]</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>www.pressebox.de/pressemitteilung/wunderlich-gmbh/Noch-mehr-Spass-an-der-Kurve/boxid/1058973</t>
+          <t>https://www.reiser-st.com/joint-press-release-on-successful-easa-level-d-qualification-of-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulator-at-norwegian-competence-centre-helicopter-as-ncch/</t>
         </is>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2021.5.14 - 10:03</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1122,30 +1056,26 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Neue FAL in Toulouse</t>
+          <t>Airbus Defence and Space selects Reiser Simulation and Training for the Provision of Eurofighter Synthetic Training System Cockpits Replacement</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Airbus schafft in Hamburg Platz für die A321XLR</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>HAMBURG - Der Airbus-Verkaufsschlager A321neo soll von Ende 2022 an auch am Firmensitz im südfranzösischen Toulouse zusammengebaut werden. Airbus rechnet wieder mit steigender Nachfrage im Brot-und-Butter-Programm. Das ist nicht der einzige Grund für die Einrichtung der neuen Linie.»</t>
-        </is>
-      </c>
+          <t>Berg, Germany, October 12, 2020 – Today’s aviation training requirements are changing, especially in the field of synthetic pilot training. The German MOD has contracted Airbus Defence and Space to extend the Eurofighter/Typhoon Pilot Synthetic Training System (PSTS) at the Main Operating Base (MOB) in Laage and introduce state-of-the-art simulator cockpits at all Eurofighter MOBs […]</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39633/Airbus-schafft-in-Hamburg-Platz-fuer-die-A321XLR.html</t>
+          <t>https://www.reiser-st.com/airbus-defence-and-space-selects-reiser-simulation-and-training-for-the-provision-of-eurofighter-synthetic-training-system-cockpits-replacement/</t>
         </is>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2021.5.14 - 7:33</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1156,30 +1086,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sicherheit</t>
+          <t>2021-02 RHT/UWETS Asia</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Airlines setzen Flüge nach Tel Aviv aus</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>FRANKFURT / TEL AVIV - Die Lufthansa setzt wegen der Eskalation im Gaza-Konflikt ihre Flüge nach Tel Aviv bis mindestens diesen Freitag aus. Auch British Airlines und alle großen US-Fluggesellschaften haben wegen des neu aufgeflammten Nahost-Konflikts alle Flüge von und nach Tel Aviv annulliert.»</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>www.aero.de/news-39631/Lufthansa-setzt-Fluege-nach-Tel-Aviv-aus.html</t>
-        </is>
-      </c>
+          <t>We are proud to announce a repeat order for a combined Rescue Hoist and Under Water Escape Training System. The order was placed by the South-East Asian customer who ordered the same system in October last year. We would like to thank them for their great confidence after the short period of cooperation.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2021.5.14 - 7:33</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1190,30 +1112,26 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Neue FAL in Toulouse</t>
+          <t>2021-02 Normobaric Hypoxia Acceptance</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Airbus schafft in Hamburg Platz für die A321XLR</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>HAMBURG - Der Airbus-Verkaufsschlager A321neo soll von Ende 2022 an auch am Firmensitz im südfranzösischen Toulouse zusammengebaut werden. Airbus rechnet wieder mit steigender Nachfrage im Brot-und-Butter-Programm. Das ist jedoch nicht der einzige Grund für die Einrichtung der neuen Linie.»</t>
-        </is>
-      </c>
+          <t>AMST successfully handed over two Reduced Oxygen Breathing Devices (ROBDs) for normobaric hypoxia training to two of its AIRFOX customers. The devices are part of upgrades to existing AIRFOX ASD and AIRFOX DISO systems.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39633/Airbus-schafft-in-Hamburg-Platz-fuer-die-A321XLR.html</t>
+          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2021-02-normobaric-hypoxia-acceptance-162/</t>
         </is>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2021.5.14 - 8:03</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1224,31 +1142,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Erstes Bauteil von AeroComposite geliefert</t>
+          <t>2020-12 Charity Donation</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Russischer Kohlefaserflügel für MS-21</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Airbus arbeitet in Toulouse an einer modernisierten...</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>https://shop.motorpresse.de/flugrevue/abo/abo-fur-mich/?hnr=extern.verlag.flugrevue.navigation</t>
-        </is>
-      </c>
+          <t>Already in early autumn, the staff at our headquarters in Ranshofen decided to donate to a charitable cause instead of having a Christmas party. It was very important to the employees to support people in need living around the company location in these difficult times. The amount of 4350 Euros was given to two charities: The Children’s Cancer Help Organisation for Upper Austria and Braunau Life Aid.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2021.5.14 - 11:03</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
@@ -1259,33 +1168,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Testprogramm gleich bei Großübung in Alaska</t>
+          <t>2020-11 Engl Flightteam Cooperation</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-F-15EX fliegt bei „Northern Edge“</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Airbus arbeitet in Toulouse an einer modernisierten...</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>https://shop.motorpresse.de/flugrevue/abo/abo-fur-mich/?hnr=extern.verlag.flugrevue.navigation</t>
-        </is>
-      </c>
+          <t>Engl Flightteam, a flight training provider, signed a partnership agreement with AMST in October 2020. The cooperation focusses on Spatial Disorientation training on our AIRFOX ASD and Multi Crew Coordination (MCC) training on our newly qualified AIRFOX UPRT simulator. We wish all trainees a great time at AMST and an excellent experience with our simulation equipment.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2021.5.14 - 11:03</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1296,31 +1194,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Nachnutzung der A380-Anlagen</t>
+          <t>2020-11-18 COVID Situation Update</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Neue A320-Montagelinie in Toulouse</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Airbus arbeitet in Toulouse an einer modernisierten...</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Dear Business Partners and Colleagues!
+Austria’s government implemented a hard lockdown starting 17 November 2020 to curb COVID infection rates. AMST has already demonstrated during the first lockdown in Spring that it has the necessary structures, tools and – most importantly – the determination to ensure continuity and success of its business. </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://shop.motorpresse.de/flugrevue/abo/abo-fur-mich/?hnr=extern.verlag.flugrevue.navigation</t>
+          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2020-11-18-covid-situation-update-156/</t>
         </is>
       </c>
       <c r="F27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2021.5.14 - 11:03</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
@@ -1331,30 +1225,26 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sicherheit</t>
+          <t>2020-11 RHT/UWETS Asia</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Airlines setzen Flüge nach Tel Aviv aus</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>FRANKFURT / TEL AVIV - Die Lufthansa setzt wegen der Eskalation im Gaza-Konflikt ihre Flüge nach Tel Aviv bis mindestens diesen Freitag aus. Auch British Airways, Wizz Air und alle großen US-Fluggesellschaften haben wegen des neu aufgeflammten Nahost-Konflikts alle Flüge von und nach Tel Aviv annulliert.»</t>
-        </is>
-      </c>
+          <t>AMST’s leading role for Rescue Hoist Training was underlined by a second contract for a Rescue Hoist Trainer (RHT) within the year 2020 from a South-East Asian Training Organisation. The contract also includes a complete Underwater Egress Training System (UWETS) with parachute training equipment.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39631/Lufthansa-setzt-Fluege-nach-Tel-Aviv-aus.html</t>
+          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2020-11-rhtuwets-asia-155/</t>
         </is>
       </c>
       <c r="F28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2021.5.14 - 11:33</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1365,30 +1255,26 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sicherheit</t>
+          <t>2021-02 FFS UPRT Upgrade</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>EASA warnt vor Flügen im israelischen Luftraum</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>TEL AVIV - Israel hat am Freitagmorgen Luftangriffe auf Hamas-Stellungen in Gaza geflogen und erstmals Bodentruppen eingesetzt. Hamas-Kämpfer feuerten erneut Raketen auf israelisches Gebiet ab. Die europäische Luftfahrtaufsicht EASA warnt vor Gefahren für den zivilen Luftverkehr in der Region.»</t>
-        </is>
-      </c>
+          <t>We are pleased to announce an additional contract award placed in January 2021. This extensive software upgrade, including UPRT to an in-service FFS, will be implemented and completed in just 12 weeks.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39638/EASA-warnt-vor-Fluegen-im-israelischen-Luftraum.html</t>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2021-02-ffs-uprt-upgrade-164/</t>
         </is>
       </c>
       <c r="F29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2021.5.14 - 13:03</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1399,33 +1285,26 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Schweizer Turboprop</t>
+          <t>2020-11 AMST at GATS-V 2020</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Pilatus liefert 1800. PC-12 aus</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Embraer hat mit der Aerodata AG aus Braunschweig einen Vertrag über den Kauf einer Praetor 600 unterzeichnet. Der Business Jet soll 2022...</t>
-        </is>
-      </c>
+          <t>AMST participates in the Global Airline Training &amp; Simulation (GATS) Virtual Conference and Tradeshow taking place from 10-12 Nov. 2020. You can visit our virtual booth at www.gats-event.com. We are looking forward to present to you our ground-breaking solutions for best quality pilot training.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.aerokurier.de</t>
+          <t>https://www.amst.co.athttps://www.gats-event.com</t>
         </is>
       </c>
       <c r="F30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2021.5.14 - 14:33</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -1436,33 +1315,26 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Schweizer Turboprop</t>
+          <t>2020-07 AMST now on YouTube</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Pilatus liefert 1800. PC-12 aus</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Pilatus hat den 1800. PC-12 an einen Kunden übergeben. Neuer...</t>
-        </is>
-      </c>
+          <t>AMST is now on YouTube with videos in HD and playlists for our business units. Enjoy, share and subscribe to our channel to stay updated!</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.aerokurier.de/business-aviation/schweizer-turboprop-pilatus-liefert-1800-pc-12-aus/</t>
+          <t>https://www.amst.co.athttps://www.youtube.com/channel/UCOKLkJRlI2MLPagBC-3gCIg/playlists</t>
         </is>
       </c>
       <c r="F31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2021.5.14 - 14:33</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -1473,30 +1345,26 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sicherheit</t>
+          <t>2020-06 AIRFOX UPRT Qualification</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Lufthansa verlängert Flugstopp nach Israel</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>FRANKFURT - Angesichts des militärischen Konflikts in Israel hat die Lufthansa-Gruppe weitere Flüge in die Region gestrichen.»</t>
-        </is>
-      </c>
+          <t>AMST is delighted to announce the qualification of our intermediate training device as a Generic Multi Engine Turbofan Aeroplane FNPT II MCC by EASA.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>www.aero.de/news-39641/Lufthansa-verlaengert-Flugstopp-nach-Israel.html</t>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-06-airfox-uprt-qualification-147/</t>
         </is>
       </c>
       <c r="F32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2021.5.14 - 16:33</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -1507,18 +1375,19 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sikorsky and Rheinmetall continue to count on German industrial team: Reiser strengthens education and training of maintenance staff</t>
+          <t>2020-04-21 CEO Message</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>January 27, 2021 Heavy-lift helicopter: Sikorsky and Rheinmetall expand German industrial partnership on CH-53K Teaming agreement renewed: Sikorsky and Rheinmetall continue to count on German industrial team Bavarian Mittelstand company Reiser strengthens education and training of maintenance staff Berlin/Düsseldorf/Berg, January 27, 2021 – Sikorsky and the members of the German CH-53K industry team have reaffirmed […]</t>
+          <t xml:space="preserve">Dear Customers, Partners, Suppliers and Colleagues!
+As we are already in the 6th week under COVID restrictions, I would like to say a big „Thank You!“ to all of you for taking the highest effort to run a more or less regular business together! </t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.reiser-st.com/sikorsky-and-rheinmetall-continue-to-count-on-german-industrial-team-reiser-strengthens-education-and-training-of-maintenance-staff/</t>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-04-21-ceo-message-143/</t>
         </is>
       </c>
       <c r="F33" t="b">
@@ -1526,7 +1395,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -1537,18 +1406,18 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Joint Press Release on Successful EASA Level D Qualification of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator at Norwegian Competence Centre Helicopter AS (NCCH)</t>
+          <t>2020-03-17 Corona Virus Situation</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Berg, Germany / Stavanger, Norway, October 8, 2020 Last week the first-of-its-kind H135 (EC135 T3H) full flight simulator was initially qualified as to the highest standard Level D by the responsible competent aviation authority CAA Norway. Therefore the simulator is now available for training under European Aviation Safety Agency (EASA) regulations. This simulator is a […]</t>
+          <t xml:space="preserve">A message from the AMST Group's CEO regarding the current Corona virus situation. </t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.reiser-st.com/joint-press-release-on-successful-easa-level-d-qualification-of-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulator-at-norwegian-competence-centre-helicopter-as-ncch/</t>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-03-17-corona-virus-situation-140/</t>
         </is>
       </c>
       <c r="F34" t="b">
@@ -1556,7 +1425,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
@@ -1567,18 +1436,18 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Airbus Defence and Space selects Reiser Simulation and Training for the Provision of Eurofighter Synthetic Training System Cockpits Replacement</t>
+          <t>2019-10 AIRFOX FFS Level D Qualification</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Berg, Germany, October 12, 2020 – Today’s aviation training requirements are changing, especially in the field of synthetic pilot training. The German MOD has contracted Airbus Defence and Space to extend the Eurofighter/Typhoon Pilot Synthetic Training System (PSTS) at the Main Operating Base (MOB) in Laage and introduce state-of-the-art simulator cockpits at all Eurofighter MOBs […]</t>
+          <t xml:space="preserve">AMST is delighted to announce the qualification of our first A320 NEO Full Flight Simulator (White Tail) to an EASA CS-FSTD(A)-Issue 2 Level D standard. This Full Flight Simulator was designed and built by AMST Aviation BV, at our facility in the Netherlands (close to Schiphol Airport). </t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.reiser-st.com/airbus-defence-and-space-selects-reiser-simulation-and-training-for-the-provision-of-eurofighter-synthetic-training-system-cockpits-replacement/</t>
+          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2019-10-airfox-ffs-level-d-qualification-124/</t>
         </is>
       </c>
       <c r="F35" t="b">
@@ -1586,7 +1455,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -1597,12 +1466,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2021-02 RHT/UWETS Asia</t>
+          <t>2019-10 EATS Berlin</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>We are proud to announce a repeat order for a combined Rescue Hoist and Under Water Escape Training System. The order was placed by the South-East Asian customer who ordered the same system in October last year. We would like to thank them for their great confidence after the short period of cooperation.</t>
+          <t>AMST-Aviation will participate in the European Airline Training Symposium (EATS), which takes place from 29-30 October 2019 in Berlin. Visit us at our booth 114 to discuss with our CEO, CTO and other subject matter experts the exciting solutions AMST-Aviation offers for your training needs.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -1612,7 +1481,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
@@ -1623,26 +1492,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2021-02 Normobaric Hypoxia Acceptance</t>
+          <t>2019-09 APATS Singapore</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AMST successfully handed over two Reduced Oxygen Breathing Devices (ROBDs) for normobaric hypoxia training to two of its AIRFOX customers. The devices are part of upgrades to existing AIRFOX ASD and AIRFOX DISO systems.</t>
+          <t>AMST-Aviation will participate in the Asia Pacific Airline Training Summit (APATS), which takes place from 3-4 September 2019 at the Sands Expo Convention centre in Singapore. Visit us at our booth 201 to discuss with our CEO, CTO and other subject matter experts the exciting solutions AMST-Aviation offers for your training needs.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2021-02-normobaric-hypoxia-acceptance-162/</t>
-        </is>
-      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -1653,12 +1518,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2020-12 Charity Donation</t>
+          <t>2019-05 WATS Orlando</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Already in early autumn, the staff at our headquarters in Ranshofen decided to donate to a charitable cause instead of having a Christmas party. It was very important to the employees to support people in need living around the company location in these difficult times. The amount of 4350 Euros was given to two charities: The Children’s Cancer Help Organisation for Upper Austria and Braunau Life Aid.</t>
+          <t>AMST will participate at WATS 2019 in Orlando, USA. We are looking forward to meeting with worldwide leading airlines and training organisations. If you are interested in talking to us at the conference, please contact us via e-mail office@amst-aviation.com or use the conference app.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -1668,7 +1533,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.5.17 - 13:44</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
@@ -1679,22 +1544,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2020-11 Engl Flightteam Cooperation</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Engl Flightteam, a flight training provider, signed a partnership agreement with AMST in October 2020. The cooperation focusses on Spatial Disorientation training on our AIRFOX ASD and Multi Crew Coordination (MCC) training on our newly qualified AIRFOX UPRT simulator. We wish all trainees a great time at AMST and an excellent experience with our simulation equipment.</t>
-        </is>
-      </c>
+          <t>["[' - ETC Awarded Contract from the University of North Dakota’s John D. Odegard School of Aerospace Sciences', "]</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>https://www.etcusa.com/etc-awarded-contract-from-the-university-of-north-dakotas-john-d-odegard-school-of-aerospace-sciences/</t>
+        </is>
+      </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -1705,19 +1570,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2020-11-18 COVID Situation Update</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Dear Business Partners and Colleagues!
-Austria’s government implemented a hard lockdown starting 17 November 2020 to curb COVID infection rates. AMST has already demonstrated during the first lockdown in Spring that it has the necessary structures, tools and – most importantly – the determination to ensure continuity and success of its business. </t>
-        </is>
-      </c>
+          <t>["[' - ETC Announces Notice of Annual Meeting of Shareholders', "]</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2020-11-18-covid-situation-update-156/</t>
+          <t>https://www.etcusa.com/etc-announces-notice-of-annual-meeting-of-shareholders-2/</t>
         </is>
       </c>
       <c r="F40" t="b">
@@ -1725,7 +1585,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -1736,18 +1596,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2020-11 RHT/UWETS Asia</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>AMST’s leading role for Rescue Hoist Training was underlined by a second contract for a Rescue Hoist Trainer (RHT) within the year 2020 from a South-East Asian Training Organisation. The contract also includes a complete Underwater Egress Training System (UWETS) with parachute training equipment.</t>
-        </is>
-      </c>
+          <t>["[' ETC Announces Fiscal 2022 Second Quarter Results', "]</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/aerospace-medicine/corporate-menu/news-events/2020-11-rhtuwets-asia-155/</t>
+          <t>https://www.etcusa.com/etc-announces-fiscal-2022-second-quarter-results/</t>
         </is>
       </c>
       <c r="F41" t="b">
@@ -1755,7 +1611,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
@@ -1766,18 +1622,18 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2021-02 FFS UPRT Upgrade</t>
+          <t>Reiser Simulation and Training teams up with RS Flight Systems to provide new product line on FNPTs and FTDs to the helicpoter training market</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>We are pleased to announce an additional contract award placed in January 2021. This extensive software upgrade, including UPRT to an in-service FFS, will be implemented and completed in just 12 weeks.</t>
+          <t>Berg, Germany, 30.09.2021 Reiser Simulation and Training GmbH (RST) has teamed up with RS Flight Systems GmbH (RSFS) to provide innovative and cost-effective FNPT and FTD products to the market. The new product line called “F-light line” for “Flightsimulator light” will feature the well-proven Level D capable flight model together with the Helionix® avionics replica, […]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2021-02-ffs-uprt-upgrade-164/</t>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-teams-up-with-rs-flight-systems-to-provide-new-product-line-on-fnpts-andftds-to-the-helicpoter-training-market/</t>
         </is>
       </c>
       <c r="F42" t="b">
@@ -1785,7 +1641,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -1796,18 +1652,18 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2020-11 AMST at GATS-V 2020</t>
+          <t>Reiser Simulation and Training GmbH to Expand Helicopter Full Flight Simulator Portfolio</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>AMST participates in the Global Airline Training &amp; Simulation (GATS) Virtual Conference and Tradeshow taking place from 10-12 Nov. 2020. You can visit our virtual booth at www.gats-event.com. We are looking forward to present to you our ground-breaking solutions for best quality pilot training.</t>
+          <t>Berg, Germany, September 16, 2021 Reiser Simulation and Training GmbH (RST) expands its portfolio of innovative flight training solutions. The German simulator manufacturer is proud of having welcomed Swiss Air-Rescue (Rega) and Leonardo Helicopters to its headquarters for the signing of their latest contract. RST has been awarded a contract from Rega for the provision […]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.amst.co.athttps://www.gats-event.com</t>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-to-expand-helicopter-full-flight-simulator-portfolio/</t>
         </is>
       </c>
       <c r="F43" t="b">
@@ -1815,7 +1671,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -1826,18 +1682,18 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2020-07 AMST now on YouTube</t>
+          <t>Successful EASA Level D Qualification&lt;br&gt;of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator&lt;br&gt;at Lufthansa Aviation Training GmbH (LAT)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>AMST is now on YouTube with videos in HD and playlists for our business units. Enjoy, share and subscribe to our channel to stay updated!</t>
+          <t>Berg / Frankfurt a. Main / Germany, May 31, 2021 RST’s newest Airbus H135 full flight simulator was initially qualified to the highest standard Level D by the German Federal Aviation Office (Luftfahrt-Bundesamt / LBA) according to European Aviation Safety Agency (EASA) regulations. The most modern FFS helicopter type H135 is thus ready for training […]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.amst.co.athttps://www.youtube.com/channel/UCOKLkJRlI2MLPagBC-3gCIg/playlists</t>
+          <t>https://www.reiser-st.com/successful-easa-level-d-qualificationof-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulatorat-lufthansa-aviation-training-gmbh-lat/</t>
         </is>
       </c>
       <c r="F44" t="b">
@@ -1845,7 +1701,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -1856,18 +1712,27 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2020-06 AIRFOX UPRT Qualification</t>
+          <t xml:space="preserve">
+RHT/UWETS Asia Repeat Order </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>AMST is delighted to announce the qualification of our intermediate training device as a Generic Multi Engine Turbofan Aeroplane FNPT II MCC by EASA.</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr"/>
+          <t xml:space="preserve">
+				News				
+2021-02-15 
+</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			We are proud to announce a repeat order for a combined Rescue Hoist and Under Water Escape Training System. The...		</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-06-airfox-uprt-qualification-147/</t>
+          <t>https://www.amst.co.at/news-aerospace-medicine/rht-uwets-asia-repeat-order/</t>
         </is>
       </c>
       <c r="F45" t="b">
@@ -1875,7 +1740,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -1886,19 +1751,27 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2020-04-21 CEO Message</t>
+          <t xml:space="preserve">
+Normobaric Hypoxia Acceptance </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dear Customers, Partners, Suppliers and Colleagues!
-As we are already in the 6th week under COVID restrictions, I would like to say a big „Thank You!“ to all of you for taking the highest effort to run a more or less regular business together! </t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr"/>
+          <t xml:space="preserve">
+				News				
+2021-02-09 
+</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			AMST successfully handed over two Reduced Oxygen Breathing Devices (ROBDs) for normobaric hypoxia training to two of its AIRFOX customers....		</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-04-21-ceo-message-143/</t>
+          <t>https://www.amst.co.at/news-aerospace-medicine/normobaric-hypoxia-acceptance/</t>
         </is>
       </c>
       <c r="F46" t="b">
@@ -1906,7 +1779,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -1917,18 +1790,27 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2020-03-17 Corona Virus Situation</t>
+          <t xml:space="preserve">
+Charity Donation </t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">A message from the AMST Group's CEO regarding the current Corona virus situation. </t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr"/>
+          <t xml:space="preserve">
+				News				
+2020-12-16 
+</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			Already in early autumn, the staff at our headquarters in Ranshofen decided to donate to a charitable cause instead of...		</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2020-03-17-corona-virus-situation-140/</t>
+          <t>https://www.amst.co.at/news-aerospace-medicine/charity-donation/</t>
         </is>
       </c>
       <c r="F47" t="b">
@@ -1936,7 +1818,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -1947,18 +1829,27 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2019-10 AIRFOX FFS Level D Qualification</t>
+          <t xml:space="preserve">
+AMST at WATS 2021 </t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMST is delighted to announce the qualification of our first A320 NEO Full Flight Simulator (White Tail) to an EASA CS-FSTD(A)-Issue 2 Level D standard. This Full Flight Simulator was designed and built by AMST Aviation BV, at our facility in the Netherlands (close to Schiphol Airport). </t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr"/>
+          <t xml:space="preserve">
+				News				
+2021-06-11 
+</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			AMST is participating in the World Aviation Training Summit (WATS) taking place on 15 and 16 of June 2021 in Orlando Florida. Join us at our booth #223 to have...		</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/en/civil-aviation/corporate-menu/news-events/2019-10-airfox-ffs-level-d-qualification-124/</t>
+          <t>https://www.amst.co.at/news-civil-aviation/amst-at-wats-2021/</t>
         </is>
       </c>
       <c r="F48" t="b">
@@ -1966,7 +1857,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -1977,22 +1868,35 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2019-10 EATS Berlin</t>
+          <t xml:space="preserve">
+FFS UPRT Upgrade </t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>AMST-Aviation will participate in the European Airline Training Symposium (EATS), which takes place from 29-30 October 2019 in Berlin. Visit us at our booth 114 to discuss with our CEO, CTO and other subject matter experts the exciting solutions AMST-Aviation offers for your training needs.</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+          <t xml:space="preserve">
+				News				
+2021-02-15 
+</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			Upset Prevention and Recovery Training (UPRT) remains a crucial topic in our industry. AMST has developed and delivered a range of solutions to this demanding requirement. We have applied almost...		</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-civil-aviation/ffs-uprt-upgrade/</t>
+        </is>
+      </c>
       <c r="F49" t="b">
         <v>0</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -2003,22 +1907,35 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2019-09 APATS Singapore</t>
+          <t xml:space="preserve">
+Engl Flightteam Cooperation </t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AMST-Aviation will participate in the Asia Pacific Airline Training Summit (APATS), which takes place from 3-4 September 2019 at the Sands Expo Convention centre in Singapore. Visit us at our booth 201 to discuss with our CEO, CTO and other subject matter experts the exciting solutions AMST-Aviation offers for your training needs.</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
+          <t xml:space="preserve">
+				News				
+2020-11-20 
+</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+			Engl Flightteam, a flight training provider, signed a partnership agreement with AMST in October 2020. The cooperation focusses on Spatial Disorientation training on our AIRFOX ASD and Multi Crew Coordination...		</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>https://www.amst.co.at/news-aerospace-medicine/engl-flightteam-cooperation/</t>
+        </is>
+      </c>
       <c r="F50" t="b">
         <v>0</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -2029,22 +1946,27 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2019-05 WATS Orlando</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>AMST will participate at WATS 2019 in Orlando, USA. We are looking forward to meeting with worldwide leading airlines and training organisations. If you are interested in talking to us at the conference, please contact us via e-mail office@amst-aviation.com or use the conference app.</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+          <t>Drei auf einen Streich - herzlichen Glückwunsch</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Erfolgreiche bestandene Prüfung dreier Schüler
+...</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/105-umschulung-ppl-auf-ul-malte-3</t>
+        </is>
+      </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2021.5.17 - 15:29</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
@@ -2055,27 +1977,27 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Die Bell 525 hat einen ersten Flug mit SAF absolviert                            
-premium</t>
+          <t>Täglich grüßt das Murmeltier</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Nachdem Bell Textron seit März 2021 nachhaltig produzierten Treibstoff (SAF) für seine eigene Vorführ- und Trainingsflotte nutzt, hat der Hersteller nun bekanntgegeben, […]</t>
+          <t>Schon wieder 100 Stunden geflogen!
+...</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://aerobuzz.de/helikopter/die-bell-525-hat-einen-ersten-flug-mit-saf-absolviert/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/103-taeglich-gruesst-das-murmeltier</t>
         </is>
       </c>
       <c r="F52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -2086,14 +2008,19 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>["[' - ETC Awarded Contract from the University of North Dakota’s John D. Odegard School of Aerospace Sciences', "]</t>
+          <t>Wenn die Flugschule zu den Schülern fliegt !</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 
+...</t>
+        </is>
+      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-awarded-contract-from-the-university-of-north-dakotas-john-d-odegard-school-of-aerospace-sciences/</t>
+          <t>https://www.flighttraining-service.de//aktuelles/blog/102-wenn-die-flugschule-zu-den-schuelern-fliegt</t>
         </is>
       </c>
       <c r="F53" t="b">
@@ -2101,7 +2028,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -2112,14 +2039,15 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>["[' - ETC Announces Notice of Annual Meeting of Shareholders', "]</t>
+          <t>Nächster verfügbarer PPL Abendkurs
+    14. Februar 2022</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-announces-notice-of-annual-meeting-of-shareholders-2/</t>
+          <t>http://www.fliegerverein.eu/abendkurs.htm</t>
         </is>
       </c>
       <c r="F54" t="b">
@@ -2127,7 +2055,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
@@ -2138,14 +2066,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>["[' ETC Announces Fiscal 2022 Second Quarter Results', "]</t>
+          <t xml:space="preserve">MFA Fernlehrgänge 2021 – garantiert “Viren Frei”
+buchbar als  “NUR THEORIEAUSBILDUNG”  NEU: Nahunterricht mit Video System (Zoom)
+</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://www.etcusa.com/etc-announces-fiscal-2022-second-quarter-results/</t>
+          <t>https://www.mfa.aero/de/</t>
         </is>
       </c>
       <c r="F55" t="b">
@@ -2153,7 +2083,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
@@ -2164,18 +2094,20 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Reiser Simulation and Training teams up with RS Flight Systems to provide new product line on FNPTs and FTDs to the helicpoter training market</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Berg, Germany, 30.09.2021 Reiser Simulation and Training GmbH (RST) has teamed up with RS Flight Systems GmbH (RSFS) to provide innovative and cost-effective FNPT and FTD products to the market. The new product line called “F-light line” for “Flightsimulator light” will feature the well-proven Level D capable flight model together with the Helionix® avionics replica, […]</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Wir sind für Sie da !  Sie erreichen uns jederzeit email:  info@mfa.aero
+Tel +49 89 642 707 61  –  Tel +49 821 747 24 60 
+– Theorieschulung über distance learning – ZFU genehmigt !
+Covid-19 Antigen Schnelltests bei MFA verfügbar !
+MFA setzt HEPA Filter nach den Infektionsschutzmaßnahmen ein.
+! Starten Sie jetzt Ihre Ausbildung !
+</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://www.reiser-st.com/reiser-simulation-and-training-teams-up-with-rs-flight-systems-to-provide-new-product-line-on-fnpts-andftds-to-the-helicpoter-training-market/</t>
+          <t>https://www.mfa.aero/de/</t>
         </is>
       </c>
       <c r="F56" t="b">
@@ -2183,7 +2115,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -2192,20 +2124,22 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Reiser Simulation and Training GmbH to Expand Helicopter Full Flight Simulator Portfolio</t>
-        </is>
-      </c>
+      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Berg, Germany, September 16, 2021 Reiser Simulation and Training GmbH (RST) expands its portfolio of innovative flight training solutions. The German simulator manufacturer is proud of having welcomed Swiss Air-Rescue (Rega) and Leonardo Helicopters to its headquarters for the signing of their latest contract. RST has been awarded a contract from Rega for the provision […]</t>
+          <t>Start your Flight Training NOW and be ready for Take Off when the post-COVID-19 Aviation-Boom Sets in!
+Thinking about becoming an airline pilot and getting your Airline Transport Pilot License?
+Get on your career track with us:
+Request free information material now!
+Apply now and be part of our next ‘Pilot Casting Day’! Upcoming Pilot Casting Days:
+5th February 2022
+5th March 2022</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-to-expand-helicopter-full-flight-simulator-portfolio/</t>
+          <t>https://www.eaa.aero/en/</t>
         </is>
       </c>
       <c r="F57" t="b">
@@ -2213,7 +2147,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -2222,20 +2156,22 @@
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Successful EASA Level D Qualification&lt;br&gt;of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator&lt;br&gt;at Lufthansa Aviation Training GmbH (LAT)</t>
-        </is>
-      </c>
+      <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Berg / Frankfurt a. Main / Germany, May 31, 2021 RST’s newest Airbus H135 full flight simulator was initially qualified to the highest standard Level D by the German Federal Aviation Office (Luftfahrt-Bundesamt / LBA) according to European Aviation Safety Agency (EASA) regulations. The most modern FFS helicopter type H135 is thus ready for training […]</t>
+          <t>Current Course Schedules
+Here are the upcoming dates for our integrated Airline Transport Pilot License classes that are now ready for boarding!
+21st February 2022
+2nd May 2022
+25th July 2022
+12th September 2022
+14th November 2022</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://www.reiser-st.com/successful-easa-level-d-qualificationof-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulatorat-lufthansa-aviation-training-gmbh-lat/</t>
+          <t>https://www.eaa.aero/en/</t>
         </is>
       </c>
       <c r="F58" t="b">
@@ -2243,7 +2179,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.11.25 - 11:15</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2254,27 +2190,14 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-RHT/UWETS Asia Repeat Order </t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-				News				
-2021-02-15 
-</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-			We are proud to announce a repeat order for a combined Rescue Hoist and Under Water Escape Training System. The...		</t>
-        </is>
-      </c>
+          <t>["[' ETC Awarded $1.8 Million Contract for its Sterilization Systems Group', "]</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/news-aerospace-medicine/rht-uwets-asia-repeat-order/</t>
+          <t>https://www.etcusa.com/etc-awarded-1-8-million-contract-for-its-sterilization-systems-group/</t>
         </is>
       </c>
       <c r="F59" t="b">
@@ -2282,7 +2205,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.12.27 - 18:24</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -2293,27 +2216,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Normobaric Hypoxia Acceptance </t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-				News				
-2021-02-09 
-</t>
-        </is>
-      </c>
+          <t>Reiser Simulation and Training teams up with RS Flight Systems to provide new product line on FNPTs and FTDs to the helicpoter training market</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
           <t xml:space="preserve">
-			AMST successfully handed over two Reduced Oxygen Breathing Devices (ROBDs) for normobaric hypoxia training to two of its AIRFOX customers....		</t>
+ </t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/news-aerospace-medicine/normobaric-hypoxia-acceptance/</t>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-teams-up-with-rs-flight-systems-to-provide-new-product-line-on-fnpts-andftds-to-the-helicpoter-training-market/</t>
         </is>
       </c>
       <c r="F60" t="b">
@@ -2321,7 +2236,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.12.27 - 18:24</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -2332,27 +2247,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Charity Donation </t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-				News				
-2020-12-16 
-</t>
-        </is>
-      </c>
+          <t>Reiser Simulation and Training GmbH to Expand Helicopter Full Flight Simulator Portfolio</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
           <t xml:space="preserve">
-			Already in early autumn, the staff at our headquarters in Ranshofen decided to donate to a charitable cause instead of...		</t>
+ </t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/news-aerospace-medicine/charity-donation/</t>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-to-expand-helicopter-full-flight-simulator-portfolio/</t>
         </is>
       </c>
       <c r="F61" t="b">
@@ -2360,7 +2267,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.12.27 - 18:24</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -2371,27 +2278,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-AMST at WATS 2021 </t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-				News				
-2021-06-11 
-</t>
-        </is>
-      </c>
+          <t>Successful EASA Level D Qualificationof Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulatorat Lufthansa Aviation Training GmbH (LAT)</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
           <t xml:space="preserve">
-			AMST is participating in the World Aviation Training Summit (WATS) taking place on 15 and 16 of June 2021 in Orlando Florida. Join us at our booth #223 to have...		</t>
+ </t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/news-civil-aviation/amst-at-wats-2021/</t>
+          <t>https://www.reiser-st.com/successful-easa-level-d-qualificationof-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulatorat-lufthansa-aviation-training-gmbh-lat/</t>
         </is>
       </c>
       <c r="F62" t="b">
@@ -2399,7 +2298,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.12.27 - 18:24</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -2410,27 +2309,19 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-FFS UPRT Upgrade </t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-				News				
-2021-02-15 
-</t>
-        </is>
-      </c>
+          <t>Sikorsky and Rheinmetall continue to count on German industrial team: Reiser strengthens education and training of maintenance staff</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
           <t xml:space="preserve">
-			Upset Prevention and Recovery Training (UPRT) remains a crucial topic in our industry. AMST has developed and delivered a range of solutions to this demanding requirement. We have applied almost...		</t>
+ </t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://www.amst.co.at/news-civil-aviation/ffs-uprt-upgrade/</t>
+          <t>https://www.reiser-st.com/sikorsky-and-rheinmetall-continue-to-count-on-german-industrial-team-reiser-strengthens-education-and-training-of-maintenance-staff/</t>
         </is>
       </c>
       <c r="F63" t="b">
@@ -2438,7 +2329,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2021.11.25 - 15:58</t>
+          <t>2021.12.27 - 18:24</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
@@ -2449,38 +2340,395 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Engl Flightteam Cooperation </t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-				News				
-2020-11-20 
+          <t>Joint Press Release on Successful EASA Level D Qualification of Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulator at Norwegian Competence Centre Helicopter AS (NCCH)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/joint-press-release-on-successful-easa-level-d-qualification-of-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulator-at-norwegian-competence-centre-helicopter-as-ncch/</t>
+        </is>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Airbus Defence and Space selects Reiser Simulation and Training for the Provision of Eurofighter Synthetic Training System Cockpits Replacement</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/airbus-defence-and-space-selects-reiser-simulation-and-training-for-the-provision-of-eurofighter-synthetic-training-system-cockpits-replacement/</t>
+        </is>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Reiser’s H145 Full Flight Simulator @Lufthansa Aviation Training GmbH – Qualified to EASA Level D by German Federal Aviation Office</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reisers-h145-full-flight-simulator-lufthansa-aviation-training-gmbh-qualified-to-easa-level-d-by-german-federal-aviation-office/</t>
+        </is>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>CONTRACT SIGNATURE @LUFTHANSA AVIATION TRAINING GMBH</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/contract-signature-lufthansa-aviation-training-gmbh/</t>
+        </is>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Reiser Simulation and Training GmbH (RST) has been contracted by NATO Helicopter Management Agency (NAHEMA) for the delivery of a MRH90 Maintenance Training Rig for the Australian Forces</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-rst-was-contracted-by-nato-helicopter-management-agency-nahema-for-the-delivery-of-a-mrh90-maintenance-training-rig-for-the-australian-forces/</t>
+        </is>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>H125 Full-Flight Simulator Qualified by Finnish Regulatory Authority</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/h125-full-flight-simulator-qualified-by-finnish-regulatory-authority/</t>
+        </is>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Reiser Simulation and Training teams up with RS Flight Systems to provide new product line on FNPTs and FTDs to the helicpoter training market</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+von Marios Felekidis | 30. September 2021 | News | 0 KommentierenBerg, Germany, 30.09.2021 Reiser Simulation and Training GmbH (RST) has teamed up with RS Flight Systems GmbH (RSFS) to provide innovative and cost-effective FNPT and FTD products to the market. The new product line called “F-light line” for “Flightsimulator light” will feature the well-proven Level D capable flight model together with the Helionix® avionics replica, supplied by RST.Together... </t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-teams-up-with-rs-flight-systems-to-provide-new-product-line-on-fnpts-andftds-to-the-helicpoter-training-market/</t>
+        </is>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Reiser Simulation and Training GmbH announced as winner in in category Outstanding VR/AR/MR Application in MS&amp;T Industry Awards 2019</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-announced-as-winner-in-in-category-outstanding-vr-ar-mr-application-in-mst-industry-awards-2019/</t>
+        </is>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Reiser Simulation and Training GmbH to Expand Helicopter Full Flight Simulator Portfolio</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+von Marios Felekidis | 20. September 2021 | News | 0 KommentierenBerg, Germany, September 16, 2021 Reiser Simulation and Training GmbH (RST) expands its portfolio of innovative flight training solutions. The German simulator manufacturer is proud of having welcomed Swiss Air-Rescue (Rega) and Leonardo Helicopters to its headquarters for the signing of their latest contract. RST has been awarded a contract from Rega for the provision of a multi-platform Level... </t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/reiser-simulation-and-training-gmbh-to-expand-helicopter-full-flight-simulator-portfolio/</t>
+        </is>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Ceremonial Handover of NTH90 MTR FC Maintenance Training Rig to the German Navy Air Wing 5 in Nordholz, Lower Saxony</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ </t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/ceremonial-handover-of-nth90-mtr-fc-maintenance-training-rig-to-the-german-navy-air-wing-5-in-nordholz-lower-saxony/</t>
+        </is>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Successful EASA Level D Qualificationof Reiser Simulation and Training GmbH (RST) H135 Full Flight Simulatorat Lufthansa Aviation Training GmbH (LAT)</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+von Marios Felekidis | 31. Mai 2021 | News | 0 KommentierenBerg / Frankfurt a. Main / Germany, May 31, 2021 RST’s newest Airbus H135 full flight simulator was initially qualified to the highest standard Level D by the German Federal Aviation Office (Luftfahrt-Bundesamt / LBA) according to European Aviation Safety Agency (EASA) regulations. The most modern FFS helicopter type H135 is thus ready for training at the major training location of Lufthansa... </t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://www.reiser-st.com/successful-easa-level-d-qualificationof-reiser-simulation-and-training-gmbh-rst-h135-full-flight-simulatorat-lufthansa-aviation-training-gmbh-lat/</t>
+        </is>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Nächster Fluglehrerkurs
+    20. September 2022</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>http://www.fliegerverein.eu/fluglehrer.htm</t>
+        </is>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MFA Fernlehrgänge 2022 – garantiert “Viren Frei”
+buchbar als  “NUR THEORIEAUSBILDUNG”  NEU: Nahunterricht mit Video System (Zoom)
 </t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-			Engl Flightteam, a flight training provider, signed a partnership agreement with AMST in October 2020. The cooperation focusses on Spatial Disorientation training on our AIRFOX ASD and Multi Crew Coordination...		</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>https://www.amst.co.at/news-aerospace-medicine/engl-flightteam-cooperation/</t>
-        </is>
-      </c>
-      <c r="F64" t="b">
-        <v>0</v>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>2021.11.25 - 15:58</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://www.mfa.aero/de/</t>
+        </is>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2021.12.27 - 18:24</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>